<commit_message>
Began Imputing Missing Values (Titanic 3.0.0)
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C676667E-B837-4B27-A6AD-77589CD9DDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E557008-948A-4CC8-8648-54FFABA510EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Titanic 1.0" sheetId="1" r:id="rId1"/>
     <sheet name="Titanic 2.0" sheetId="2" r:id="rId2"/>
-    <sheet name="Pipelines" sheetId="3" r:id="rId3"/>
-    <sheet name="Alert" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="Ideas" sheetId="5" r:id="rId5"/>
+    <sheet name="Titanic 3.0" sheetId="6" r:id="rId3"/>
+    <sheet name="Pipelines" sheetId="3" r:id="rId4"/>
+    <sheet name="Alert" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Ideas" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
   <si>
     <t>Version</t>
   </si>
@@ -250,6 +252,33 @@
   </si>
   <si>
     <t>Completed pie charts on Lone, Spent, VIP, CryoSleep</t>
+  </si>
+  <si>
+    <t>Titanic 2.0.6</t>
+  </si>
+  <si>
+    <t>2024 08 07</t>
+  </si>
+  <si>
+    <t>Feature Extraction: AgeGroup, FamilySize. Saved feature engineered datasets as train and test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need to impute missing data before some accumulated data: AgeGroup, FamilySize, Spent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need to impute missing data first. I will redo this file. </t>
+  </si>
+  <si>
+    <t>Titanic 3.0.0</t>
+  </si>
+  <si>
+    <t>Moved to Titanic 3.0.0. to deal with missing values using Titanic 1.0.2</t>
+  </si>
+  <si>
+    <t>Created from Titanic 1.0.2</t>
+  </si>
+  <si>
+    <t>Stopped at Imputing Home Planet Missing Values.</t>
   </si>
 </sst>
 </file>
@@ -818,7 +847,7 @@
   <dimension ref="A1:L986"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,24 +923,36 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3967,8 +4008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L986"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4074,10 +4115,18 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -7131,6 +7180,3141 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
+  <dimension ref="A1:L986"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="141" customWidth="1"/>
+    <col min="5" max="6" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" customWidth="1"/>
+    <col min="8" max="1025" width="8.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="5"/>
+      <c r="D24" s="3"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="5"/>
+      <c r="D26" s="3"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="5"/>
+      <c r="D27" s="3"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="5"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="5"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="5"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="5"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="5"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="3"/>
+      <c r="B34" s="5"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" s="3"/>
+      <c r="B36" s="5"/>
+      <c r="D36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="5"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B40" s="5"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B41" s="5"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B42" s="5"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B43" s="5"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B44" s="5"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B45" s="5"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B46" s="5"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D116" s="3"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D118" s="3"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D120" s="3"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D129" s="3"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D130" s="3"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D132" s="3"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D135" s="3"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D136" s="3"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D147" s="3"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D148" s="3"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D149" s="3"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D150" s="3"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D157" s="3"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D159" s="3"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D161" s="3"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D183" s="3"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D190" s="3"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D191" s="3"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D209" s="3"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D210" s="3"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D211" s="3"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D212" s="3"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D213" s="3"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D214" s="3"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D215" s="3"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D218" s="3"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D219" s="3"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D220" s="3"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D221" s="3"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D222" s="3"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D223" s="3"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D224" s="3"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D225" s="3"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D226" s="3"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D227" s="3"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D228" s="3"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D229" s="3"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D230" s="3"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D231" s="3"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D232" s="3"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D233" s="3"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D234" s="3"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D235" s="3"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D236" s="3"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D237" s="3"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D238" s="3"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D240" s="3"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D241" s="3"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D242" s="3"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D243" s="3"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D244" s="3"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D245" s="3"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D246" s="3"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D247" s="3"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D248" s="3"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D249" s="3"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D251" s="3"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D252" s="3"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D253" s="3"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D254" s="3"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D255" s="3"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D256" s="3"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D257" s="3"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D258" s="3"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D259" s="3"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D260" s="3"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D261" s="3"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D262" s="3"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D263" s="3"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D264" s="3"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D265" s="3"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D266" s="3"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D267" s="3"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D268" s="3"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D269" s="3"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D270" s="3"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D271" s="3"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D272" s="3"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D273" s="3"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D274" s="3"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D275" s="3"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D276" s="3"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D277" s="3"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D278" s="3"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D279" s="3"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D280" s="3"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D281" s="3"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D282" s="3"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D283" s="3"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D284" s="3"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D285" s="3"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D286" s="3"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D287" s="3"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D288" s="3"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D289" s="3"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D290" s="3"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D291" s="3"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D292" s="3"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D293" s="3"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D294" s="3"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D295" s="3"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D296" s="3"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D297" s="3"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D298" s="3"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D299" s="3"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D300" s="3"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D301" s="3"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D302" s="3"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D303" s="3"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D304" s="3"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D305" s="3"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D306" s="3"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D307" s="3"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D308" s="3"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D309" s="3"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D310" s="3"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D311" s="3"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D312" s="3"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D313" s="3"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D314" s="3"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D315" s="3"/>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D316" s="3"/>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D317" s="3"/>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D318" s="3"/>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D319" s="3"/>
+    </row>
+    <row r="320" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D320" s="3"/>
+    </row>
+    <row r="321" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D321" s="3"/>
+    </row>
+    <row r="322" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D322" s="3"/>
+    </row>
+    <row r="323" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D323" s="3"/>
+    </row>
+    <row r="324" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D324" s="3"/>
+    </row>
+    <row r="325" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D325" s="3"/>
+    </row>
+    <row r="326" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D326" s="3"/>
+    </row>
+    <row r="327" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D327" s="3"/>
+    </row>
+    <row r="328" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D328" s="3"/>
+    </row>
+    <row r="329" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D329" s="3"/>
+    </row>
+    <row r="330" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D330" s="3"/>
+    </row>
+    <row r="331" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D331" s="3"/>
+    </row>
+    <row r="332" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D332" s="3"/>
+    </row>
+    <row r="333" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D333" s="3"/>
+    </row>
+    <row r="334" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D334" s="3"/>
+    </row>
+    <row r="335" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D335" s="3"/>
+    </row>
+    <row r="336" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D336" s="3"/>
+    </row>
+    <row r="337" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D337" s="3"/>
+    </row>
+    <row r="338" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D338" s="3"/>
+    </row>
+    <row r="339" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D339" s="3"/>
+    </row>
+    <row r="340" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D340" s="3"/>
+    </row>
+    <row r="341" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D341" s="3"/>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D342" s="3"/>
+    </row>
+    <row r="343" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D343" s="3"/>
+    </row>
+    <row r="344" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D344" s="3"/>
+    </row>
+    <row r="345" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D345" s="3"/>
+    </row>
+    <row r="346" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D346" s="3"/>
+    </row>
+    <row r="347" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D347" s="3"/>
+    </row>
+    <row r="348" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D348" s="3"/>
+    </row>
+    <row r="349" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D349" s="3"/>
+    </row>
+    <row r="350" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D350" s="3"/>
+    </row>
+    <row r="351" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D351" s="3"/>
+    </row>
+    <row r="352" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D352" s="3"/>
+    </row>
+    <row r="353" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D353" s="3"/>
+    </row>
+    <row r="354" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D354" s="3"/>
+    </row>
+    <row r="355" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D355" s="3"/>
+    </row>
+    <row r="356" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D356" s="3"/>
+    </row>
+    <row r="357" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D357" s="3"/>
+    </row>
+    <row r="358" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D358" s="3"/>
+    </row>
+    <row r="359" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D359" s="3"/>
+    </row>
+    <row r="360" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D360" s="3"/>
+    </row>
+    <row r="361" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D361" s="3"/>
+    </row>
+    <row r="362" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D362" s="3"/>
+    </row>
+    <row r="363" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D363" s="3"/>
+    </row>
+    <row r="364" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D364" s="3"/>
+    </row>
+    <row r="365" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D365" s="3"/>
+    </row>
+    <row r="366" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D366" s="3"/>
+    </row>
+    <row r="367" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D367" s="3"/>
+    </row>
+    <row r="368" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D368" s="3"/>
+    </row>
+    <row r="369" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D369" s="3"/>
+    </row>
+    <row r="370" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D370" s="3"/>
+    </row>
+    <row r="371" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D371" s="3"/>
+    </row>
+    <row r="372" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D372" s="3"/>
+    </row>
+    <row r="373" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D373" s="3"/>
+    </row>
+    <row r="374" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D374" s="3"/>
+    </row>
+    <row r="375" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D375" s="3"/>
+    </row>
+    <row r="376" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D376" s="3"/>
+    </row>
+    <row r="377" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D377" s="3"/>
+    </row>
+    <row r="378" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D378" s="3"/>
+    </row>
+    <row r="379" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D379" s="3"/>
+    </row>
+    <row r="380" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D380" s="3"/>
+    </row>
+    <row r="381" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D381" s="3"/>
+    </row>
+    <row r="382" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D382" s="3"/>
+    </row>
+    <row r="383" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D383" s="3"/>
+    </row>
+    <row r="384" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D384" s="3"/>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D385" s="3"/>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D386" s="3"/>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D387" s="3"/>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D388" s="3"/>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D389" s="3"/>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D390" s="3"/>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D391" s="3"/>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D392" s="3"/>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D393" s="3"/>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D394" s="3"/>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D395" s="3"/>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D396" s="3"/>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D397" s="3"/>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D398" s="3"/>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D399" s="3"/>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D400" s="3"/>
+    </row>
+    <row r="401" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D401" s="3"/>
+    </row>
+    <row r="402" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D402" s="3"/>
+    </row>
+    <row r="403" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D403" s="3"/>
+    </row>
+    <row r="404" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D404" s="3"/>
+    </row>
+    <row r="405" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D405" s="3"/>
+    </row>
+    <row r="406" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D406" s="3"/>
+    </row>
+    <row r="407" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D407" s="3"/>
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D408" s="3"/>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D409" s="3"/>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D410" s="3"/>
+    </row>
+    <row r="411" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D411" s="3"/>
+    </row>
+    <row r="412" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D412" s="3"/>
+    </row>
+    <row r="413" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D413" s="3"/>
+    </row>
+    <row r="414" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D414" s="3"/>
+    </row>
+    <row r="415" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D415" s="3"/>
+    </row>
+    <row r="416" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D416" s="3"/>
+    </row>
+    <row r="417" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D417" s="3"/>
+    </row>
+    <row r="418" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D418" s="3"/>
+    </row>
+    <row r="419" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D419" s="3"/>
+    </row>
+    <row r="420" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D420" s="3"/>
+    </row>
+    <row r="421" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D421" s="3"/>
+    </row>
+    <row r="422" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D422" s="3"/>
+    </row>
+    <row r="423" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D423" s="3"/>
+    </row>
+    <row r="424" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D424" s="3"/>
+    </row>
+    <row r="425" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D425" s="3"/>
+    </row>
+    <row r="426" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D426" s="3"/>
+    </row>
+    <row r="427" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D427" s="3"/>
+    </row>
+    <row r="428" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D428" s="3"/>
+    </row>
+    <row r="429" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D429" s="3"/>
+    </row>
+    <row r="430" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D430" s="3"/>
+    </row>
+    <row r="431" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D431" s="3"/>
+    </row>
+    <row r="432" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D432" s="3"/>
+    </row>
+    <row r="433" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D433" s="3"/>
+    </row>
+    <row r="434" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D434" s="3"/>
+    </row>
+    <row r="435" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D435" s="3"/>
+    </row>
+    <row r="436" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D436" s="3"/>
+    </row>
+    <row r="437" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D437" s="3"/>
+    </row>
+    <row r="438" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D438" s="3"/>
+    </row>
+    <row r="439" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D439" s="3"/>
+    </row>
+    <row r="440" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D440" s="3"/>
+    </row>
+    <row r="441" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D441" s="3"/>
+    </row>
+    <row r="442" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D442" s="3"/>
+    </row>
+    <row r="443" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D443" s="3"/>
+    </row>
+    <row r="444" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D444" s="3"/>
+    </row>
+    <row r="445" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D445" s="3"/>
+    </row>
+    <row r="446" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D446" s="3"/>
+    </row>
+    <row r="447" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D447" s="3"/>
+    </row>
+    <row r="448" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D448" s="3"/>
+    </row>
+    <row r="449" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D449" s="3"/>
+    </row>
+    <row r="450" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D450" s="3"/>
+    </row>
+    <row r="451" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D451" s="3"/>
+    </row>
+    <row r="452" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D452" s="3"/>
+    </row>
+    <row r="453" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D453" s="3"/>
+    </row>
+    <row r="454" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D454" s="3"/>
+    </row>
+    <row r="455" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D455" s="3"/>
+    </row>
+    <row r="456" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D456" s="3"/>
+    </row>
+    <row r="457" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D457" s="3"/>
+    </row>
+    <row r="458" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D458" s="3"/>
+    </row>
+    <row r="459" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D459" s="3"/>
+    </row>
+    <row r="460" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D460" s="3"/>
+    </row>
+    <row r="461" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D461" s="3"/>
+    </row>
+    <row r="462" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D462" s="3"/>
+    </row>
+    <row r="463" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D463" s="3"/>
+    </row>
+    <row r="464" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D464" s="3"/>
+    </row>
+    <row r="465" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D465" s="3"/>
+    </row>
+    <row r="466" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D466" s="3"/>
+    </row>
+    <row r="467" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D467" s="3"/>
+    </row>
+    <row r="468" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D468" s="3"/>
+    </row>
+    <row r="469" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D469" s="3"/>
+    </row>
+    <row r="470" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D470" s="3"/>
+    </row>
+    <row r="471" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D471" s="3"/>
+    </row>
+    <row r="472" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D472" s="3"/>
+    </row>
+    <row r="473" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D473" s="3"/>
+    </row>
+    <row r="474" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D474" s="3"/>
+    </row>
+    <row r="475" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D475" s="3"/>
+    </row>
+    <row r="476" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D476" s="3"/>
+    </row>
+    <row r="477" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D477" s="3"/>
+    </row>
+    <row r="478" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D478" s="3"/>
+    </row>
+    <row r="479" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D479" s="3"/>
+    </row>
+    <row r="480" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D480" s="3"/>
+    </row>
+    <row r="481" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D481" s="3"/>
+    </row>
+    <row r="482" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D482" s="3"/>
+    </row>
+    <row r="483" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D483" s="3"/>
+    </row>
+    <row r="484" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D484" s="3"/>
+    </row>
+    <row r="485" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D485" s="3"/>
+    </row>
+    <row r="486" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D486" s="3"/>
+    </row>
+    <row r="487" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D487" s="3"/>
+    </row>
+    <row r="488" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D488" s="3"/>
+    </row>
+    <row r="489" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D489" s="3"/>
+    </row>
+    <row r="490" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D490" s="3"/>
+    </row>
+    <row r="491" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D491" s="3"/>
+    </row>
+    <row r="492" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D492" s="3"/>
+    </row>
+    <row r="493" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D493" s="3"/>
+    </row>
+    <row r="494" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D494" s="3"/>
+    </row>
+    <row r="495" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D495" s="3"/>
+    </row>
+    <row r="496" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D496" s="3"/>
+    </row>
+    <row r="497" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D497" s="3"/>
+    </row>
+    <row r="498" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D498" s="3"/>
+    </row>
+    <row r="499" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D499" s="3"/>
+    </row>
+    <row r="500" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D500" s="3"/>
+    </row>
+    <row r="501" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D501" s="3"/>
+    </row>
+    <row r="502" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D502" s="3"/>
+    </row>
+    <row r="503" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D503" s="3"/>
+    </row>
+    <row r="504" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D504" s="3"/>
+    </row>
+    <row r="505" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D505" s="3"/>
+    </row>
+    <row r="506" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D506" s="3"/>
+    </row>
+    <row r="507" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D507" s="3"/>
+    </row>
+    <row r="508" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D508" s="3"/>
+    </row>
+    <row r="509" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D509" s="3"/>
+    </row>
+    <row r="510" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D510" s="3"/>
+    </row>
+    <row r="511" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D511" s="3"/>
+    </row>
+    <row r="512" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D512" s="3"/>
+    </row>
+    <row r="513" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D513" s="3"/>
+    </row>
+    <row r="514" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D514" s="3"/>
+    </row>
+    <row r="515" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D515" s="3"/>
+    </row>
+    <row r="516" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D516" s="3"/>
+    </row>
+    <row r="517" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D517" s="3"/>
+    </row>
+    <row r="518" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D518" s="3"/>
+    </row>
+    <row r="519" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D519" s="3"/>
+    </row>
+    <row r="520" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D520" s="3"/>
+    </row>
+    <row r="521" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D521" s="3"/>
+    </row>
+    <row r="522" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D522" s="3"/>
+    </row>
+    <row r="523" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D523" s="3"/>
+    </row>
+    <row r="524" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D524" s="3"/>
+    </row>
+    <row r="525" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D525" s="3"/>
+    </row>
+    <row r="526" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D526" s="3"/>
+    </row>
+    <row r="527" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D527" s="3"/>
+    </row>
+    <row r="528" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D528" s="3"/>
+    </row>
+    <row r="529" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D529" s="3"/>
+    </row>
+    <row r="530" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D530" s="3"/>
+    </row>
+    <row r="531" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D531" s="3"/>
+    </row>
+    <row r="532" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D532" s="3"/>
+    </row>
+    <row r="533" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D533" s="3"/>
+    </row>
+    <row r="534" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D534" s="3"/>
+    </row>
+    <row r="535" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D535" s="3"/>
+    </row>
+    <row r="536" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D536" s="3"/>
+    </row>
+    <row r="537" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D537" s="3"/>
+    </row>
+    <row r="538" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D538" s="3"/>
+    </row>
+    <row r="539" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D539" s="3"/>
+    </row>
+    <row r="540" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D540" s="3"/>
+    </row>
+    <row r="541" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D541" s="3"/>
+    </row>
+    <row r="542" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D542" s="3"/>
+    </row>
+    <row r="543" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D543" s="3"/>
+    </row>
+    <row r="544" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D544" s="3"/>
+    </row>
+    <row r="545" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D545" s="3"/>
+    </row>
+    <row r="546" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D546" s="3"/>
+    </row>
+    <row r="547" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D547" s="3"/>
+    </row>
+    <row r="548" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D548" s="3"/>
+    </row>
+    <row r="549" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D549" s="3"/>
+    </row>
+    <row r="550" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D550" s="3"/>
+    </row>
+    <row r="551" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D551" s="3"/>
+    </row>
+    <row r="552" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D552" s="3"/>
+    </row>
+    <row r="553" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D553" s="3"/>
+    </row>
+    <row r="554" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D554" s="3"/>
+    </row>
+    <row r="555" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D555" s="3"/>
+    </row>
+    <row r="556" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D556" s="3"/>
+    </row>
+    <row r="557" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D557" s="3"/>
+    </row>
+    <row r="558" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D558" s="3"/>
+    </row>
+    <row r="559" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D559" s="3"/>
+    </row>
+    <row r="560" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D560" s="3"/>
+    </row>
+    <row r="561" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D561" s="3"/>
+    </row>
+    <row r="562" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D562" s="3"/>
+    </row>
+    <row r="563" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D563" s="3"/>
+    </row>
+    <row r="564" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D564" s="3"/>
+    </row>
+    <row r="565" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D565" s="3"/>
+    </row>
+    <row r="566" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D566" s="3"/>
+    </row>
+    <row r="567" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D567" s="3"/>
+    </row>
+    <row r="568" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D568" s="3"/>
+    </row>
+    <row r="569" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D569" s="3"/>
+    </row>
+    <row r="570" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D570" s="3"/>
+    </row>
+    <row r="571" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D571" s="3"/>
+    </row>
+    <row r="572" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D572" s="3"/>
+    </row>
+    <row r="573" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D573" s="3"/>
+    </row>
+    <row r="574" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D574" s="3"/>
+    </row>
+    <row r="575" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D575" s="3"/>
+    </row>
+    <row r="576" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D576" s="3"/>
+    </row>
+    <row r="577" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D577" s="3"/>
+    </row>
+    <row r="578" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D578" s="3"/>
+    </row>
+    <row r="579" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D579" s="3"/>
+    </row>
+    <row r="580" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D580" s="3"/>
+    </row>
+    <row r="581" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D581" s="3"/>
+    </row>
+    <row r="582" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D582" s="3"/>
+    </row>
+    <row r="583" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D583" s="3"/>
+    </row>
+    <row r="584" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D584" s="3"/>
+    </row>
+    <row r="585" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D585" s="3"/>
+    </row>
+    <row r="586" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D586" s="3"/>
+    </row>
+    <row r="587" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D587" s="3"/>
+    </row>
+    <row r="588" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D588" s="3"/>
+    </row>
+    <row r="589" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D589" s="3"/>
+    </row>
+    <row r="590" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D590" s="3"/>
+    </row>
+    <row r="591" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D591" s="3"/>
+    </row>
+    <row r="592" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D592" s="3"/>
+    </row>
+    <row r="593" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D593" s="3"/>
+    </row>
+    <row r="594" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D594" s="3"/>
+    </row>
+    <row r="595" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D595" s="3"/>
+    </row>
+    <row r="596" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D596" s="3"/>
+    </row>
+    <row r="597" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D597" s="3"/>
+    </row>
+    <row r="598" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D598" s="3"/>
+    </row>
+    <row r="599" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D599" s="3"/>
+    </row>
+    <row r="600" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D600" s="3"/>
+    </row>
+    <row r="601" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D601" s="3"/>
+    </row>
+    <row r="602" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D602" s="3"/>
+    </row>
+    <row r="603" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D603" s="3"/>
+    </row>
+    <row r="604" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D604" s="3"/>
+    </row>
+    <row r="605" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D605" s="3"/>
+    </row>
+    <row r="606" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D606" s="3"/>
+    </row>
+    <row r="607" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D607" s="3"/>
+    </row>
+    <row r="608" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D608" s="3"/>
+    </row>
+    <row r="609" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D609" s="3"/>
+    </row>
+    <row r="610" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D610" s="3"/>
+    </row>
+    <row r="611" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D611" s="3"/>
+    </row>
+    <row r="612" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D612" s="3"/>
+    </row>
+    <row r="613" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D613" s="3"/>
+    </row>
+    <row r="614" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D614" s="3"/>
+    </row>
+    <row r="615" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D615" s="3"/>
+    </row>
+    <row r="616" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D616" s="3"/>
+    </row>
+    <row r="617" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D617" s="3"/>
+    </row>
+    <row r="618" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D618" s="3"/>
+    </row>
+    <row r="619" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D619" s="3"/>
+    </row>
+    <row r="620" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D620" s="3"/>
+    </row>
+    <row r="621" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D621" s="3"/>
+    </row>
+    <row r="622" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D622" s="3"/>
+    </row>
+    <row r="623" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D623" s="3"/>
+    </row>
+    <row r="624" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D624" s="3"/>
+    </row>
+    <row r="625" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D625" s="3"/>
+    </row>
+    <row r="626" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D626" s="3"/>
+    </row>
+    <row r="627" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D627" s="3"/>
+    </row>
+    <row r="628" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D628" s="3"/>
+    </row>
+    <row r="629" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D629" s="3"/>
+    </row>
+    <row r="630" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D630" s="3"/>
+    </row>
+    <row r="631" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D631" s="3"/>
+    </row>
+    <row r="632" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D632" s="3"/>
+    </row>
+    <row r="633" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D633" s="3"/>
+    </row>
+    <row r="634" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D634" s="3"/>
+    </row>
+    <row r="635" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D635" s="3"/>
+    </row>
+    <row r="636" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D636" s="3"/>
+    </row>
+    <row r="637" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D637" s="3"/>
+    </row>
+    <row r="638" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D638" s="3"/>
+    </row>
+    <row r="639" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D639" s="3"/>
+    </row>
+    <row r="640" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D640" s="3"/>
+    </row>
+    <row r="641" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D641" s="3"/>
+    </row>
+    <row r="642" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D642" s="3"/>
+    </row>
+    <row r="643" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D643" s="3"/>
+    </row>
+    <row r="644" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D644" s="3"/>
+    </row>
+    <row r="645" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D645" s="3"/>
+    </row>
+    <row r="646" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D646" s="3"/>
+    </row>
+    <row r="647" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D647" s="3"/>
+    </row>
+    <row r="648" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D648" s="3"/>
+    </row>
+    <row r="649" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D649" s="3"/>
+    </row>
+    <row r="650" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D650" s="3"/>
+    </row>
+    <row r="651" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D651" s="3"/>
+    </row>
+    <row r="652" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D652" s="3"/>
+    </row>
+    <row r="653" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D653" s="3"/>
+    </row>
+    <row r="654" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D654" s="3"/>
+    </row>
+    <row r="655" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D655" s="3"/>
+    </row>
+    <row r="656" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D656" s="3"/>
+    </row>
+    <row r="657" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D657" s="3"/>
+    </row>
+    <row r="658" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D658" s="3"/>
+    </row>
+    <row r="659" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D659" s="3"/>
+    </row>
+    <row r="660" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D660" s="3"/>
+    </row>
+    <row r="661" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D661" s="3"/>
+    </row>
+    <row r="662" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D662" s="3"/>
+    </row>
+    <row r="663" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D663" s="3"/>
+    </row>
+    <row r="664" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D664" s="3"/>
+    </row>
+    <row r="665" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D665" s="3"/>
+    </row>
+    <row r="666" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D666" s="3"/>
+    </row>
+    <row r="667" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D667" s="3"/>
+    </row>
+    <row r="668" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D668" s="3"/>
+    </row>
+    <row r="669" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D669" s="3"/>
+    </row>
+    <row r="670" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D670" s="3"/>
+    </row>
+    <row r="671" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D671" s="3"/>
+    </row>
+    <row r="672" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D672" s="3"/>
+    </row>
+    <row r="673" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D673" s="3"/>
+    </row>
+    <row r="674" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D674" s="3"/>
+    </row>
+    <row r="675" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D675" s="3"/>
+    </row>
+    <row r="676" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D676" s="3"/>
+    </row>
+    <row r="677" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D677" s="3"/>
+    </row>
+    <row r="678" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D678" s="3"/>
+    </row>
+    <row r="679" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D679" s="3"/>
+    </row>
+    <row r="680" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D680" s="3"/>
+    </row>
+    <row r="681" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D681" s="3"/>
+    </row>
+    <row r="682" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D682" s="3"/>
+    </row>
+    <row r="683" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D683" s="3"/>
+    </row>
+    <row r="684" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D684" s="3"/>
+    </row>
+    <row r="685" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D685" s="3"/>
+    </row>
+    <row r="686" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D686" s="3"/>
+    </row>
+    <row r="687" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D687" s="3"/>
+    </row>
+    <row r="688" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D688" s="3"/>
+    </row>
+    <row r="689" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D689" s="3"/>
+    </row>
+    <row r="690" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D690" s="3"/>
+    </row>
+    <row r="691" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D691" s="3"/>
+    </row>
+    <row r="692" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D692" s="3"/>
+    </row>
+    <row r="693" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D693" s="3"/>
+    </row>
+    <row r="694" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D694" s="3"/>
+    </row>
+    <row r="695" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D695" s="3"/>
+    </row>
+    <row r="696" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D696" s="3"/>
+    </row>
+    <row r="697" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D697" s="3"/>
+    </row>
+    <row r="698" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D698" s="3"/>
+    </row>
+    <row r="699" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D699" s="3"/>
+    </row>
+    <row r="700" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D700" s="3"/>
+    </row>
+    <row r="701" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D701" s="3"/>
+    </row>
+    <row r="702" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D702" s="3"/>
+    </row>
+    <row r="703" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D703" s="3"/>
+    </row>
+    <row r="704" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D704" s="3"/>
+    </row>
+    <row r="705" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D705" s="3"/>
+    </row>
+    <row r="706" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D706" s="3"/>
+    </row>
+    <row r="707" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D707" s="3"/>
+    </row>
+    <row r="708" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D708" s="3"/>
+    </row>
+    <row r="709" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D709" s="3"/>
+    </row>
+    <row r="710" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D710" s="3"/>
+    </row>
+    <row r="711" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D711" s="3"/>
+    </row>
+    <row r="712" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D712" s="3"/>
+    </row>
+    <row r="713" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D713" s="3"/>
+    </row>
+    <row r="714" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D714" s="3"/>
+    </row>
+    <row r="715" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D715" s="3"/>
+    </row>
+    <row r="716" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D716" s="3"/>
+    </row>
+    <row r="717" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D717" s="3"/>
+    </row>
+    <row r="718" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D718" s="3"/>
+    </row>
+    <row r="719" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D719" s="3"/>
+    </row>
+    <row r="720" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D720" s="3"/>
+    </row>
+    <row r="721" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D721" s="3"/>
+    </row>
+    <row r="722" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D722" s="3"/>
+    </row>
+    <row r="723" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D723" s="3"/>
+    </row>
+    <row r="724" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D724" s="3"/>
+    </row>
+    <row r="725" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D725" s="3"/>
+    </row>
+    <row r="726" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D726" s="3"/>
+    </row>
+    <row r="727" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D727" s="3"/>
+    </row>
+    <row r="728" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D728" s="3"/>
+    </row>
+    <row r="729" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D729" s="3"/>
+    </row>
+    <row r="730" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D730" s="3"/>
+    </row>
+    <row r="731" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D731" s="3"/>
+    </row>
+    <row r="732" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D732" s="3"/>
+    </row>
+    <row r="733" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D733" s="3"/>
+    </row>
+    <row r="734" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D734" s="3"/>
+    </row>
+    <row r="735" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D735" s="3"/>
+    </row>
+    <row r="736" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D736" s="3"/>
+    </row>
+    <row r="737" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D737" s="3"/>
+    </row>
+    <row r="738" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D738" s="3"/>
+    </row>
+    <row r="739" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D739" s="3"/>
+    </row>
+    <row r="740" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D740" s="3"/>
+    </row>
+    <row r="741" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D741" s="3"/>
+    </row>
+    <row r="742" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D742" s="3"/>
+    </row>
+    <row r="743" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D743" s="3"/>
+    </row>
+    <row r="744" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D744" s="3"/>
+    </row>
+    <row r="745" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D745" s="3"/>
+    </row>
+    <row r="746" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D746" s="3"/>
+    </row>
+    <row r="747" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D747" s="3"/>
+    </row>
+    <row r="748" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D748" s="3"/>
+    </row>
+    <row r="749" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D749" s="3"/>
+    </row>
+    <row r="750" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D750" s="3"/>
+    </row>
+    <row r="751" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D751" s="3"/>
+    </row>
+    <row r="752" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D752" s="3"/>
+    </row>
+    <row r="753" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D753" s="3"/>
+    </row>
+    <row r="754" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D754" s="3"/>
+    </row>
+    <row r="755" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D755" s="3"/>
+    </row>
+    <row r="756" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D756" s="3"/>
+    </row>
+    <row r="757" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D757" s="3"/>
+    </row>
+    <row r="758" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D758" s="3"/>
+    </row>
+    <row r="759" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D759" s="3"/>
+    </row>
+    <row r="760" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D760" s="3"/>
+    </row>
+    <row r="761" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D761" s="3"/>
+    </row>
+    <row r="762" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D762" s="3"/>
+    </row>
+    <row r="763" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D763" s="3"/>
+    </row>
+    <row r="764" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D764" s="3"/>
+    </row>
+    <row r="765" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D765" s="3"/>
+    </row>
+    <row r="766" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D766" s="3"/>
+    </row>
+    <row r="767" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D767" s="3"/>
+    </row>
+    <row r="768" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D768" s="3"/>
+    </row>
+    <row r="769" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D769" s="3"/>
+    </row>
+    <row r="770" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D770" s="3"/>
+    </row>
+    <row r="771" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D771" s="3"/>
+    </row>
+    <row r="772" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D772" s="3"/>
+    </row>
+    <row r="773" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D773" s="3"/>
+    </row>
+    <row r="774" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D774" s="3"/>
+    </row>
+    <row r="775" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D775" s="3"/>
+    </row>
+    <row r="776" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D776" s="3"/>
+    </row>
+    <row r="777" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D777" s="3"/>
+    </row>
+    <row r="778" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D778" s="3"/>
+    </row>
+    <row r="779" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D779" s="3"/>
+    </row>
+    <row r="780" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D780" s="3"/>
+    </row>
+    <row r="781" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D781" s="3"/>
+    </row>
+    <row r="782" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D782" s="3"/>
+    </row>
+    <row r="783" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D783" s="3"/>
+    </row>
+    <row r="784" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D784" s="3"/>
+    </row>
+    <row r="785" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D785" s="3"/>
+    </row>
+    <row r="786" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D786" s="3"/>
+    </row>
+    <row r="787" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D787" s="3"/>
+    </row>
+    <row r="788" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D788" s="3"/>
+    </row>
+    <row r="789" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D789" s="3"/>
+    </row>
+    <row r="790" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D790" s="3"/>
+    </row>
+    <row r="791" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D791" s="3"/>
+    </row>
+    <row r="792" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D792" s="3"/>
+    </row>
+    <row r="793" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D793" s="3"/>
+    </row>
+    <row r="794" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D794" s="3"/>
+    </row>
+    <row r="795" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D795" s="3"/>
+    </row>
+    <row r="796" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D796" s="3"/>
+    </row>
+    <row r="797" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D797" s="3"/>
+    </row>
+    <row r="798" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D798" s="3"/>
+    </row>
+    <row r="799" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D799" s="3"/>
+    </row>
+    <row r="800" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D800" s="3"/>
+    </row>
+    <row r="801" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D801" s="3"/>
+    </row>
+    <row r="802" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D802" s="3"/>
+    </row>
+    <row r="803" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D803" s="3"/>
+    </row>
+    <row r="804" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D804" s="3"/>
+    </row>
+    <row r="805" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D805" s="3"/>
+    </row>
+    <row r="806" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D806" s="3"/>
+    </row>
+    <row r="807" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D807" s="3"/>
+    </row>
+    <row r="808" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D808" s="3"/>
+    </row>
+    <row r="809" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D809" s="3"/>
+    </row>
+    <row r="810" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D810" s="3"/>
+    </row>
+    <row r="811" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D811" s="3"/>
+    </row>
+    <row r="812" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D812" s="3"/>
+    </row>
+    <row r="813" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D813" s="3"/>
+    </row>
+    <row r="814" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D814" s="3"/>
+    </row>
+    <row r="815" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D815" s="3"/>
+    </row>
+    <row r="816" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D816" s="3"/>
+    </row>
+    <row r="817" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D817" s="3"/>
+    </row>
+    <row r="818" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D818" s="3"/>
+    </row>
+    <row r="819" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D819" s="3"/>
+    </row>
+    <row r="820" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D820" s="3"/>
+    </row>
+    <row r="821" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D821" s="3"/>
+    </row>
+    <row r="822" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D822" s="3"/>
+    </row>
+    <row r="823" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D823" s="3"/>
+    </row>
+    <row r="824" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D824" s="3"/>
+    </row>
+    <row r="825" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D825" s="3"/>
+    </row>
+    <row r="826" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D826" s="3"/>
+    </row>
+    <row r="827" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D827" s="3"/>
+    </row>
+    <row r="828" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D828" s="3"/>
+    </row>
+    <row r="829" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D829" s="3"/>
+    </row>
+    <row r="830" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D830" s="3"/>
+    </row>
+    <row r="831" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D831" s="3"/>
+    </row>
+    <row r="832" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D832" s="3"/>
+    </row>
+    <row r="833" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D833" s="3"/>
+    </row>
+    <row r="834" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D834" s="3"/>
+    </row>
+    <row r="835" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D835" s="3"/>
+    </row>
+    <row r="836" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D836" s="3"/>
+    </row>
+    <row r="837" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D837" s="3"/>
+    </row>
+    <row r="838" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D838" s="3"/>
+    </row>
+    <row r="839" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D839" s="3"/>
+    </row>
+    <row r="840" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D840" s="3"/>
+    </row>
+    <row r="841" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D841" s="3"/>
+    </row>
+    <row r="842" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D842" s="3"/>
+    </row>
+    <row r="843" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D843" s="3"/>
+    </row>
+    <row r="844" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D844" s="3"/>
+    </row>
+    <row r="845" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D845" s="3"/>
+    </row>
+    <row r="846" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D846" s="3"/>
+    </row>
+    <row r="847" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D847" s="3"/>
+    </row>
+    <row r="848" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D848" s="3"/>
+    </row>
+    <row r="849" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D849" s="3"/>
+    </row>
+    <row r="850" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D850" s="3"/>
+    </row>
+    <row r="851" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D851" s="3"/>
+    </row>
+    <row r="852" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D852" s="3"/>
+    </row>
+    <row r="853" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D853" s="3"/>
+    </row>
+    <row r="854" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D854" s="3"/>
+    </row>
+    <row r="855" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D855" s="3"/>
+    </row>
+    <row r="856" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D856" s="3"/>
+    </row>
+    <row r="857" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D857" s="3"/>
+    </row>
+    <row r="858" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D858" s="3"/>
+    </row>
+    <row r="859" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D859" s="3"/>
+    </row>
+    <row r="860" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D860" s="3"/>
+    </row>
+    <row r="861" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D861" s="3"/>
+    </row>
+    <row r="862" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D862" s="3"/>
+    </row>
+    <row r="863" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D863" s="3"/>
+    </row>
+    <row r="864" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D864" s="3"/>
+    </row>
+    <row r="865" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D865" s="3"/>
+    </row>
+    <row r="866" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D866" s="3"/>
+    </row>
+    <row r="867" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D867" s="3"/>
+    </row>
+    <row r="868" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D868" s="3"/>
+    </row>
+    <row r="869" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D869" s="3"/>
+    </row>
+    <row r="870" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D870" s="3"/>
+    </row>
+    <row r="871" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D871" s="3"/>
+    </row>
+    <row r="872" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D872" s="3"/>
+    </row>
+    <row r="873" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D873" s="3"/>
+    </row>
+    <row r="874" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D874" s="3"/>
+    </row>
+    <row r="875" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D875" s="3"/>
+    </row>
+    <row r="876" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D876" s="3"/>
+    </row>
+    <row r="877" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D877" s="3"/>
+    </row>
+    <row r="878" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D878" s="3"/>
+    </row>
+    <row r="879" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D879" s="3"/>
+    </row>
+    <row r="880" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D880" s="3"/>
+    </row>
+    <row r="881" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D881" s="3"/>
+    </row>
+    <row r="882" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D882" s="3"/>
+    </row>
+    <row r="883" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D883" s="3"/>
+    </row>
+    <row r="884" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D884" s="3"/>
+    </row>
+    <row r="885" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D885" s="3"/>
+    </row>
+    <row r="886" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D886" s="3"/>
+    </row>
+    <row r="887" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D887" s="3"/>
+    </row>
+    <row r="888" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D888" s="3"/>
+    </row>
+    <row r="889" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D889" s="3"/>
+    </row>
+    <row r="890" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D890" s="3"/>
+    </row>
+    <row r="891" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D891" s="3"/>
+    </row>
+    <row r="892" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D892" s="3"/>
+    </row>
+    <row r="893" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D893" s="3"/>
+    </row>
+    <row r="894" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D894" s="3"/>
+    </row>
+    <row r="895" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D895" s="3"/>
+    </row>
+    <row r="896" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D896" s="3"/>
+    </row>
+    <row r="897" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D897" s="3"/>
+    </row>
+    <row r="898" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D898" s="3"/>
+    </row>
+    <row r="899" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D899" s="3"/>
+    </row>
+    <row r="900" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D900" s="3"/>
+    </row>
+    <row r="901" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D901" s="3"/>
+    </row>
+    <row r="902" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D902" s="3"/>
+    </row>
+    <row r="903" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D903" s="3"/>
+    </row>
+    <row r="904" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D904" s="3"/>
+    </row>
+    <row r="905" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D905" s="3"/>
+    </row>
+    <row r="906" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D906" s="3"/>
+    </row>
+    <row r="907" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D907" s="3"/>
+    </row>
+    <row r="908" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D908" s="3"/>
+    </row>
+    <row r="909" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D909" s="3"/>
+    </row>
+    <row r="910" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D910" s="3"/>
+    </row>
+    <row r="911" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D911" s="3"/>
+    </row>
+    <row r="912" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D912" s="3"/>
+    </row>
+    <row r="913" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D913" s="3"/>
+    </row>
+    <row r="914" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D914" s="3"/>
+    </row>
+    <row r="915" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D915" s="3"/>
+    </row>
+    <row r="916" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D916" s="3"/>
+    </row>
+    <row r="917" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D917" s="3"/>
+    </row>
+    <row r="918" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D918" s="3"/>
+    </row>
+    <row r="919" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D919" s="3"/>
+    </row>
+    <row r="920" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D920" s="3"/>
+    </row>
+    <row r="921" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D921" s="3"/>
+    </row>
+    <row r="922" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D922" s="3"/>
+    </row>
+    <row r="923" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D923" s="3"/>
+    </row>
+    <row r="924" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D924" s="3"/>
+    </row>
+    <row r="925" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D925" s="3"/>
+    </row>
+    <row r="926" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D926" s="3"/>
+    </row>
+    <row r="927" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D927" s="3"/>
+    </row>
+    <row r="928" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D928" s="3"/>
+    </row>
+    <row r="929" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D929" s="3"/>
+    </row>
+    <row r="930" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D930" s="3"/>
+    </row>
+    <row r="931" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D931" s="3"/>
+    </row>
+    <row r="932" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D932" s="3"/>
+    </row>
+    <row r="933" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D933" s="3"/>
+    </row>
+    <row r="934" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D934" s="3"/>
+    </row>
+    <row r="935" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D935" s="3"/>
+    </row>
+    <row r="936" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D936" s="3"/>
+    </row>
+    <row r="937" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D937" s="3"/>
+    </row>
+    <row r="938" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D938" s="3"/>
+    </row>
+    <row r="939" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D939" s="3"/>
+    </row>
+    <row r="940" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D940" s="3"/>
+    </row>
+    <row r="941" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D941" s="3"/>
+    </row>
+    <row r="942" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D942" s="3"/>
+    </row>
+    <row r="943" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D943" s="3"/>
+    </row>
+    <row r="944" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D944" s="3"/>
+    </row>
+    <row r="945" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D945" s="3"/>
+    </row>
+    <row r="946" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D946" s="3"/>
+    </row>
+    <row r="947" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D947" s="3"/>
+    </row>
+    <row r="948" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D948" s="3"/>
+    </row>
+    <row r="949" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D949" s="3"/>
+    </row>
+    <row r="950" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D950" s="3"/>
+    </row>
+    <row r="951" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D951" s="3"/>
+    </row>
+    <row r="952" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D952" s="3"/>
+    </row>
+    <row r="953" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D953" s="3"/>
+    </row>
+    <row r="954" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D954" s="3"/>
+    </row>
+    <row r="955" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D955" s="3"/>
+    </row>
+    <row r="956" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D956" s="3"/>
+    </row>
+    <row r="957" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D957" s="3"/>
+    </row>
+    <row r="958" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D958" s="3"/>
+    </row>
+    <row r="959" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D959" s="3"/>
+    </row>
+    <row r="960" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D960" s="3"/>
+    </row>
+    <row r="961" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D961" s="3"/>
+    </row>
+    <row r="962" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D962" s="3"/>
+    </row>
+    <row r="963" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D963" s="3"/>
+    </row>
+    <row r="964" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D964" s="3"/>
+    </row>
+    <row r="965" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D965" s="3"/>
+    </row>
+    <row r="966" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D966" s="3"/>
+    </row>
+    <row r="967" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D967" s="3"/>
+    </row>
+    <row r="968" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D968" s="3"/>
+    </row>
+    <row r="969" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D969" s="3"/>
+    </row>
+    <row r="970" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D970" s="3"/>
+    </row>
+    <row r="971" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D971" s="3"/>
+    </row>
+    <row r="972" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D972" s="3"/>
+    </row>
+    <row r="973" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D973" s="3"/>
+    </row>
+    <row r="974" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D974" s="3"/>
+    </row>
+    <row r="975" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D975" s="3"/>
+    </row>
+    <row r="976" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D976" s="3"/>
+    </row>
+    <row r="977" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D977" s="3"/>
+    </row>
+    <row r="978" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D978" s="3"/>
+    </row>
+    <row r="979" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D979" s="3"/>
+    </row>
+    <row r="980" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D980" s="3"/>
+    </row>
+    <row r="981" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D981" s="3"/>
+    </row>
+    <row r="982" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D982" s="3"/>
+    </row>
+    <row r="983" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D983" s="3"/>
+    </row>
+    <row r="984" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D984" s="3"/>
+    </row>
+    <row r="985" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D985" s="3"/>
+    </row>
+    <row r="986" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D986" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L985"/>
   <sheetViews>
@@ -10237,7 +13421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK64"/>
   <sheetViews>
@@ -12754,7 +15938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K1005"/>
   <sheetViews>

</xml_diff>

<commit_message>
Completed Imputing CryoSleep (3.0.2), Imputing Destination (3.0.3)
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E557008-948A-4CC8-8648-54FFABA510EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37890867-1DA4-4C3C-B751-2026A76EBF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="10200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Titanic 1.0" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
   <si>
     <t>Version</t>
   </si>
@@ -279,6 +279,39 @@
   </si>
   <si>
     <t>Stopped at Imputing Home Planet Missing Values.</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.1</t>
+  </si>
+  <si>
+    <t>2024 08 08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name Extraction, Age Group, and family size are here. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleted Age Group, Family size to deal with missing values </t>
+  </si>
+  <si>
+    <t>HomePlanet Missing Values</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.2</t>
+  </si>
+  <si>
+    <t>CryoSleept Missing Values (Strarting with 3.0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imputed Missing values with False since most passengers were False. </t>
+  </si>
+  <si>
+    <t>2024 08 09</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.3</t>
+  </si>
+  <si>
+    <t>Destination Planet. Start with Titanic 3.0.1 and use the same method as for HomePlanet.</t>
   </si>
 </sst>
 </file>
@@ -7181,10 +7214,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
-  <dimension ref="A1:L986"/>
+  <dimension ref="A1:L987"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7219,7 +7252,9 @@
       <c r="B2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
       </c>
@@ -7238,37 +7273,59 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G5" s="5"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -7279,10 +7336,16 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -7378,20 +7441,21 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="5"/>
       <c r="D25" s="3"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="3"/>
       <c r="G26" s="5"/>
     </row>
@@ -7399,17 +7463,18 @@
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
       <c r="D27" s="3"/>
-      <c r="G27" s="8"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="5"/>
       <c r="D28" s="3"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -7439,28 +7504,29 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="6"/>
+      <c r="B35" s="5"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="6"/>
       <c r="D36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+      <c r="B37" s="5"/>
       <c r="D37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="3"/>
-      <c r="B39" s="5"/>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
       <c r="B40" s="5"/>
       <c r="D40" s="3"/>
     </row>
@@ -7489,6 +7555,7 @@
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B47" s="5"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
@@ -10307,6 +10374,9 @@
     </row>
     <row r="986" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D986" s="3"/>
+    </row>
+    <row r="987" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D987" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Completed Imputing CabinDeck Values
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37890867-1DA4-4C3C-B751-2026A76EBF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9642EE8B-33C9-4FEA-8C62-3A3AA7107406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="10200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
   <si>
     <t>Version</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>Destination Planet. Start with Titanic 3.0.1 and use the same method as for HomePlanet.</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.4</t>
+  </si>
+  <si>
+    <t>Cabin Deck Imputation (Starting with Titanic 3.0.1). The imputation will be based on HomePlanets. This file contains HomePlanet imputation.</t>
+  </si>
+  <si>
+    <t>** Since we are filling CabinDeck and HomePlanet by LastName, we should Impute this first. **</t>
+  </si>
+  <si>
+    <t>** We should also imputer missing values for luxury spending with 0**</t>
   </si>
 </sst>
 </file>
@@ -7214,10 +7226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
-  <dimension ref="A1:L987"/>
+  <dimension ref="A1:L989"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7279,43 +7291,35 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -7323,28 +7327,30 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>87</v>
+      <c r="D8" s="3"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>85</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>89</v>
+      <c r="B9" s="3" t="s">
+        <v>81</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -7356,10 +7362,18 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -7370,24 +7384,36 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -7448,14 +7474,15 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
-      <c r="B25" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="6"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="G26" s="5"/>
     </row>
@@ -7467,24 +7494,27 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
-      <c r="B28" s="5"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="3"/>
-      <c r="G28" s="8"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="5"/>
       <c r="D29" s="3"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="5"/>
       <c r="D30" s="3"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -7509,32 +7539,34 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
-      <c r="B36" s="6"/>
+      <c r="B36" s="5"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="5"/>
       <c r="D37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+      <c r="B38" s="6"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="5"/>
       <c r="D39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="3"/>
-      <c r="B40" s="5"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B41" s="5"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
       <c r="B42" s="5"/>
       <c r="D42" s="3"/>
     </row>
@@ -7559,54 +7591,56 @@
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B48" s="5"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="5"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.35">
@@ -10377,6 +10411,12 @@
     </row>
     <row r="987" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D987" s="3"/>
+    </row>
+    <row r="988" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D988" s="3"/>
+    </row>
+    <row r="989" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D989" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Began Name Missing Data Imputation
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9642EE8B-33C9-4FEA-8C62-3A3AA7107406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5E2AF6-7C76-4B69-8D34-FBD1E86AEA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="10200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
   <si>
     <t>Version</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>** We should also imputer missing values for luxury spending with 0**</t>
+  </si>
+  <si>
+    <t>LastName  Missing Values (Strarting with 3.0.0)</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.5</t>
   </si>
 </sst>
 </file>
@@ -7229,7 +7235,7 @@
   <dimension ref="A1:L989"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7424,10 +7430,18 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
CabinSide Missing Values Imputed
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5E2AF6-7C76-4B69-8D34-FBD1E86AEA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A8239C-5BB3-4092-8CC4-7F3FCDA95D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="10200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Titanic 1.0" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
   <si>
     <t>Version</t>
   </si>
@@ -330,6 +330,30 @@
   </si>
   <si>
     <t>Titanic 3.0.5</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.6</t>
+  </si>
+  <si>
+    <t>2024 08 12</t>
+  </si>
+  <si>
+    <t>Make Missing values of Luxury Godds = 0  (Strarting with 3.0.0)</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.7</t>
+  </si>
+  <si>
+    <t>Cabin Side Missing Values (Strarting with 3.0.0)</t>
+  </si>
+  <si>
+    <t>Titanic 3.0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabin Number Missing Values </t>
   </si>
 </sst>
 </file>
@@ -7232,10 +7256,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
-  <dimension ref="A1:L989"/>
+  <dimension ref="A1:L993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7333,30 +7357,30 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -7364,21 +7388,17 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -7391,7 +7411,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>88</v>
@@ -7400,7 +7420,7 @@
         <v>88</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -7409,7 +7429,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -7417,30 +7437,30 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>94</v>
+      <c r="D16" s="3"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>91</v>
       </c>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G18" s="5"/>
     </row>
@@ -7448,7 +7468,9 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -7459,17 +7481,27 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -7480,17 +7512,27 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -7501,54 +7543,76 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="5"/>
-      <c r="D27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-      <c r="B30" s="5"/>
-      <c r="D30" s="3"/>
-      <c r="G30" s="8"/>
+      <c r="A30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="5"/>
       <c r="D31" s="3"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
-      <c r="B32" s="5"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="3"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="5"/>
       <c r="D33" s="3"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="5"/>
       <c r="D34" s="3"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
@@ -7563,40 +7627,44 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
-      <c r="B38" s="6"/>
+      <c r="B38" s="5"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="5"/>
       <c r="D39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="5"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="5"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="6"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
       <c r="B43" s="5"/>
       <c r="D43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B44" s="5"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B45" s="5"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
       <c r="B46" s="5"/>
       <c r="D46" s="3"/>
     </row>
@@ -7613,15 +7681,19 @@
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="5"/>
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="5"/>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="5"/>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="5"/>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.35">
@@ -10431,6 +10503,18 @@
     </row>
     <row r="989" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D989" s="3"/>
+    </row>
+    <row r="990" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D990" s="3"/>
+    </row>
+    <row r="991" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D991" s="3"/>
+    </row>
+    <row r="992" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D992" s="3"/>
+    </row>
+    <row r="993" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D993" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Imputation Home Planet, Destination, Cabin Deck Complete.
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,25 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0964B2-611C-49E6-ABD9-0A234E17941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0B9633-8104-4AC9-BA71-AE28EB818166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Titanic 1.0" sheetId="1" r:id="rId1"/>
     <sheet name="Titanic 2.0" sheetId="2" r:id="rId2"/>
     <sheet name="Titanic 3.0" sheetId="6" r:id="rId3"/>
     <sheet name="Overview 4.0" sheetId="7" r:id="rId4"/>
-    <sheet name="Preprocessing 5.0" sheetId="8" r:id="rId5"/>
-    <sheet name="Pipelines" sheetId="3" r:id="rId6"/>
-    <sheet name="Alert" sheetId="4" state="hidden" r:id="rId7"/>
-    <sheet name="Ideas" sheetId="5" r:id="rId8"/>
+    <sheet name="Preprocess 5.0" sheetId="8" r:id="rId5"/>
+    <sheet name="Missing 6.0" sheetId="9" r:id="rId6"/>
+    <sheet name="Pipelines" sheetId="3" r:id="rId7"/>
+    <sheet name="Alert" sheetId="4" state="hidden" r:id="rId8"/>
+    <sheet name="Ideas" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="7">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="8">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="6">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="7">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
   <si>
     <t>Version</t>
   </si>
@@ -397,6 +399,21 @@
   </si>
   <si>
     <t>Preprocessing  (Start Titanic 1.0.2)</t>
+  </si>
+  <si>
+    <t>Saved file data as data in the Data Folder.</t>
+  </si>
+  <si>
+    <t>Start Titanic 3.0.1 Home Planet</t>
+  </si>
+  <si>
+    <t>Start Titanic 3.0.3 Destination</t>
+  </si>
+  <si>
+    <t>Start Titanic 3.0.4 Cabin Deck</t>
+  </si>
+  <si>
+    <t>Cabin Side</t>
   </si>
 </sst>
 </file>
@@ -7301,7 +7318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
   <dimension ref="A1:L993"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -13793,10 +13810,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBBBD00-887E-4CE6-9C0B-B6A8EADE2E47}">
-  <dimension ref="A1:L993"/>
+  <dimension ref="A1:L994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13831,7 +13848,9 @@
       <c r="B2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>117</v>
       </c>
@@ -13841,14 +13860,18 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -13864,8 +13887,6 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
@@ -13873,6 +13894,8 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="5"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -14045,43 +14068,45 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="3"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="B34" s="5"/>
       <c r="D34" s="3"/>
-      <c r="G34" s="8"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="B37" s="5"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
@@ -14101,28 +14126,29 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
-      <c r="B42" s="6"/>
+      <c r="B42" s="5"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="6"/>
       <c r="D43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="3"/>
+      <c r="B44" s="5"/>
       <c r="D44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="3"/>
-      <c r="B46" s="5"/>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
       <c r="B47" s="5"/>
       <c r="D47" s="3"/>
     </row>
@@ -14151,6 +14177,7 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B54" s="5"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.35">
@@ -16969,6 +16996,9 @@
     </row>
     <row r="993" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D993" s="3"/>
+    </row>
+    <row r="994" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D994" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -16977,6 +17007,3213 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6254EBB-BCB6-46DB-AD5A-C24358141626}">
+  <dimension ref="A1:L993"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="141" customWidth="1"/>
+    <col min="5" max="6" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" customWidth="1"/>
+    <col min="8" max="1025" width="8.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="3"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="5"/>
+      <c r="D33" s="3"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" s="3"/>
+      <c r="B36" s="5"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+      <c r="B38" s="5"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="5"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="5"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="5"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
+      <c r="B43" s="5"/>
+      <c r="D43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="5"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B47" s="5"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B48" s="5"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="5"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="5"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="5"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="5"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="5"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D116" s="3"/>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D118" s="3"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D120" s="3"/>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D129" s="3"/>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D130" s="3"/>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D132" s="3"/>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D135" s="3"/>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D136" s="3"/>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D147" s="3"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D148" s="3"/>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D149" s="3"/>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D150" s="3"/>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D157" s="3"/>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D159" s="3"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D161" s="3"/>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D183" s="3"/>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D190" s="3"/>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D191" s="3"/>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D209" s="3"/>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D210" s="3"/>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D211" s="3"/>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D212" s="3"/>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D213" s="3"/>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D214" s="3"/>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D215" s="3"/>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D218" s="3"/>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D219" s="3"/>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D220" s="3"/>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D221" s="3"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D222" s="3"/>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D223" s="3"/>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D224" s="3"/>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D225" s="3"/>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D226" s="3"/>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D227" s="3"/>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D228" s="3"/>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D229" s="3"/>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D230" s="3"/>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D231" s="3"/>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D232" s="3"/>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D233" s="3"/>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D234" s="3"/>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D235" s="3"/>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D236" s="3"/>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D237" s="3"/>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D238" s="3"/>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D240" s="3"/>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D241" s="3"/>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D242" s="3"/>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D243" s="3"/>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D244" s="3"/>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D245" s="3"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D246" s="3"/>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D247" s="3"/>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D248" s="3"/>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D249" s="3"/>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D251" s="3"/>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D252" s="3"/>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D253" s="3"/>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D254" s="3"/>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D255" s="3"/>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D256" s="3"/>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D257" s="3"/>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D258" s="3"/>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D259" s="3"/>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D260" s="3"/>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D261" s="3"/>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D262" s="3"/>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D263" s="3"/>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D264" s="3"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D265" s="3"/>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D266" s="3"/>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D267" s="3"/>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D268" s="3"/>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D269" s="3"/>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D270" s="3"/>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D271" s="3"/>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D272" s="3"/>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D273" s="3"/>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D274" s="3"/>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D275" s="3"/>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D276" s="3"/>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D277" s="3"/>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D278" s="3"/>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D279" s="3"/>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D280" s="3"/>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D281" s="3"/>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D282" s="3"/>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D283" s="3"/>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D284" s="3"/>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D285" s="3"/>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D286" s="3"/>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D287" s="3"/>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D288" s="3"/>
+    </row>
+    <row r="289" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D289" s="3"/>
+    </row>
+    <row r="290" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D290" s="3"/>
+    </row>
+    <row r="291" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D291" s="3"/>
+    </row>
+    <row r="292" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D292" s="3"/>
+    </row>
+    <row r="293" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D293" s="3"/>
+    </row>
+    <row r="294" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D294" s="3"/>
+    </row>
+    <row r="295" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D295" s="3"/>
+    </row>
+    <row r="296" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D296" s="3"/>
+    </row>
+    <row r="297" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D297" s="3"/>
+    </row>
+    <row r="298" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D298" s="3"/>
+    </row>
+    <row r="299" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D299" s="3"/>
+    </row>
+    <row r="300" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D300" s="3"/>
+    </row>
+    <row r="301" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D301" s="3"/>
+    </row>
+    <row r="302" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D302" s="3"/>
+    </row>
+    <row r="303" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D303" s="3"/>
+    </row>
+    <row r="304" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D304" s="3"/>
+    </row>
+    <row r="305" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D305" s="3"/>
+    </row>
+    <row r="306" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D306" s="3"/>
+    </row>
+    <row r="307" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D307" s="3"/>
+    </row>
+    <row r="308" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D308" s="3"/>
+    </row>
+    <row r="309" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D309" s="3"/>
+    </row>
+    <row r="310" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D310" s="3"/>
+    </row>
+    <row r="311" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D311" s="3"/>
+    </row>
+    <row r="312" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D312" s="3"/>
+    </row>
+    <row r="313" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D313" s="3"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D314" s="3"/>
+    </row>
+    <row r="315" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D315" s="3"/>
+    </row>
+    <row r="316" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D316" s="3"/>
+    </row>
+    <row r="317" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D317" s="3"/>
+    </row>
+    <row r="318" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D318" s="3"/>
+    </row>
+    <row r="319" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D319" s="3"/>
+    </row>
+    <row r="320" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D320" s="3"/>
+    </row>
+    <row r="321" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D321" s="3"/>
+    </row>
+    <row r="322" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D322" s="3"/>
+    </row>
+    <row r="323" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D323" s="3"/>
+    </row>
+    <row r="324" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D324" s="3"/>
+    </row>
+    <row r="325" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D325" s="3"/>
+    </row>
+    <row r="326" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D326" s="3"/>
+    </row>
+    <row r="327" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D327" s="3"/>
+    </row>
+    <row r="328" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D328" s="3"/>
+    </row>
+    <row r="329" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D329" s="3"/>
+    </row>
+    <row r="330" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D330" s="3"/>
+    </row>
+    <row r="331" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D331" s="3"/>
+    </row>
+    <row r="332" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D332" s="3"/>
+    </row>
+    <row r="333" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D333" s="3"/>
+    </row>
+    <row r="334" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D334" s="3"/>
+    </row>
+    <row r="335" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D335" s="3"/>
+    </row>
+    <row r="336" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D336" s="3"/>
+    </row>
+    <row r="337" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D337" s="3"/>
+    </row>
+    <row r="338" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D338" s="3"/>
+    </row>
+    <row r="339" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D339" s="3"/>
+    </row>
+    <row r="340" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D340" s="3"/>
+    </row>
+    <row r="341" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D341" s="3"/>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D342" s="3"/>
+    </row>
+    <row r="343" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D343" s="3"/>
+    </row>
+    <row r="344" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D344" s="3"/>
+    </row>
+    <row r="345" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D345" s="3"/>
+    </row>
+    <row r="346" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D346" s="3"/>
+    </row>
+    <row r="347" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D347" s="3"/>
+    </row>
+    <row r="348" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D348" s="3"/>
+    </row>
+    <row r="349" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D349" s="3"/>
+    </row>
+    <row r="350" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D350" s="3"/>
+    </row>
+    <row r="351" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D351" s="3"/>
+    </row>
+    <row r="352" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D352" s="3"/>
+    </row>
+    <row r="353" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D353" s="3"/>
+    </row>
+    <row r="354" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D354" s="3"/>
+    </row>
+    <row r="355" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D355" s="3"/>
+    </row>
+    <row r="356" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D356" s="3"/>
+    </row>
+    <row r="357" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D357" s="3"/>
+    </row>
+    <row r="358" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D358" s="3"/>
+    </row>
+    <row r="359" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D359" s="3"/>
+    </row>
+    <row r="360" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D360" s="3"/>
+    </row>
+    <row r="361" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D361" s="3"/>
+    </row>
+    <row r="362" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D362" s="3"/>
+    </row>
+    <row r="363" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D363" s="3"/>
+    </row>
+    <row r="364" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D364" s="3"/>
+    </row>
+    <row r="365" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D365" s="3"/>
+    </row>
+    <row r="366" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D366" s="3"/>
+    </row>
+    <row r="367" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D367" s="3"/>
+    </row>
+    <row r="368" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D368" s="3"/>
+    </row>
+    <row r="369" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D369" s="3"/>
+    </row>
+    <row r="370" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D370" s="3"/>
+    </row>
+    <row r="371" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D371" s="3"/>
+    </row>
+    <row r="372" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D372" s="3"/>
+    </row>
+    <row r="373" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D373" s="3"/>
+    </row>
+    <row r="374" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D374" s="3"/>
+    </row>
+    <row r="375" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D375" s="3"/>
+    </row>
+    <row r="376" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D376" s="3"/>
+    </row>
+    <row r="377" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D377" s="3"/>
+    </row>
+    <row r="378" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D378" s="3"/>
+    </row>
+    <row r="379" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D379" s="3"/>
+    </row>
+    <row r="380" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D380" s="3"/>
+    </row>
+    <row r="381" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D381" s="3"/>
+    </row>
+    <row r="382" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D382" s="3"/>
+    </row>
+    <row r="383" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D383" s="3"/>
+    </row>
+    <row r="384" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D384" s="3"/>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D385" s="3"/>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D386" s="3"/>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D387" s="3"/>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D388" s="3"/>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D389" s="3"/>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D390" s="3"/>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D391" s="3"/>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D392" s="3"/>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D393" s="3"/>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D394" s="3"/>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D395" s="3"/>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D396" s="3"/>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D397" s="3"/>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D398" s="3"/>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D399" s="3"/>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D400" s="3"/>
+    </row>
+    <row r="401" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D401" s="3"/>
+    </row>
+    <row r="402" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D402" s="3"/>
+    </row>
+    <row r="403" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D403" s="3"/>
+    </row>
+    <row r="404" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D404" s="3"/>
+    </row>
+    <row r="405" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D405" s="3"/>
+    </row>
+    <row r="406" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D406" s="3"/>
+    </row>
+    <row r="407" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D407" s="3"/>
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D408" s="3"/>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D409" s="3"/>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D410" s="3"/>
+    </row>
+    <row r="411" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D411" s="3"/>
+    </row>
+    <row r="412" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D412" s="3"/>
+    </row>
+    <row r="413" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D413" s="3"/>
+    </row>
+    <row r="414" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D414" s="3"/>
+    </row>
+    <row r="415" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D415" s="3"/>
+    </row>
+    <row r="416" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D416" s="3"/>
+    </row>
+    <row r="417" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D417" s="3"/>
+    </row>
+    <row r="418" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D418" s="3"/>
+    </row>
+    <row r="419" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D419" s="3"/>
+    </row>
+    <row r="420" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D420" s="3"/>
+    </row>
+    <row r="421" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D421" s="3"/>
+    </row>
+    <row r="422" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D422" s="3"/>
+    </row>
+    <row r="423" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D423" s="3"/>
+    </row>
+    <row r="424" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D424" s="3"/>
+    </row>
+    <row r="425" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D425" s="3"/>
+    </row>
+    <row r="426" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D426" s="3"/>
+    </row>
+    <row r="427" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D427" s="3"/>
+    </row>
+    <row r="428" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D428" s="3"/>
+    </row>
+    <row r="429" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D429" s="3"/>
+    </row>
+    <row r="430" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D430" s="3"/>
+    </row>
+    <row r="431" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D431" s="3"/>
+    </row>
+    <row r="432" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D432" s="3"/>
+    </row>
+    <row r="433" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D433" s="3"/>
+    </row>
+    <row r="434" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D434" s="3"/>
+    </row>
+    <row r="435" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D435" s="3"/>
+    </row>
+    <row r="436" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D436" s="3"/>
+    </row>
+    <row r="437" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D437" s="3"/>
+    </row>
+    <row r="438" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D438" s="3"/>
+    </row>
+    <row r="439" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D439" s="3"/>
+    </row>
+    <row r="440" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D440" s="3"/>
+    </row>
+    <row r="441" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D441" s="3"/>
+    </row>
+    <row r="442" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D442" s="3"/>
+    </row>
+    <row r="443" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D443" s="3"/>
+    </row>
+    <row r="444" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D444" s="3"/>
+    </row>
+    <row r="445" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D445" s="3"/>
+    </row>
+    <row r="446" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D446" s="3"/>
+    </row>
+    <row r="447" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D447" s="3"/>
+    </row>
+    <row r="448" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D448" s="3"/>
+    </row>
+    <row r="449" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D449" s="3"/>
+    </row>
+    <row r="450" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D450" s="3"/>
+    </row>
+    <row r="451" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D451" s="3"/>
+    </row>
+    <row r="452" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D452" s="3"/>
+    </row>
+    <row r="453" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D453" s="3"/>
+    </row>
+    <row r="454" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D454" s="3"/>
+    </row>
+    <row r="455" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D455" s="3"/>
+    </row>
+    <row r="456" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D456" s="3"/>
+    </row>
+    <row r="457" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D457" s="3"/>
+    </row>
+    <row r="458" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D458" s="3"/>
+    </row>
+    <row r="459" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D459" s="3"/>
+    </row>
+    <row r="460" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D460" s="3"/>
+    </row>
+    <row r="461" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D461" s="3"/>
+    </row>
+    <row r="462" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D462" s="3"/>
+    </row>
+    <row r="463" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D463" s="3"/>
+    </row>
+    <row r="464" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D464" s="3"/>
+    </row>
+    <row r="465" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D465" s="3"/>
+    </row>
+    <row r="466" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D466" s="3"/>
+    </row>
+    <row r="467" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D467" s="3"/>
+    </row>
+    <row r="468" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D468" s="3"/>
+    </row>
+    <row r="469" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D469" s="3"/>
+    </row>
+    <row r="470" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D470" s="3"/>
+    </row>
+    <row r="471" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D471" s="3"/>
+    </row>
+    <row r="472" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D472" s="3"/>
+    </row>
+    <row r="473" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D473" s="3"/>
+    </row>
+    <row r="474" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D474" s="3"/>
+    </row>
+    <row r="475" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D475" s="3"/>
+    </row>
+    <row r="476" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D476" s="3"/>
+    </row>
+    <row r="477" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D477" s="3"/>
+    </row>
+    <row r="478" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D478" s="3"/>
+    </row>
+    <row r="479" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D479" s="3"/>
+    </row>
+    <row r="480" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D480" s="3"/>
+    </row>
+    <row r="481" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D481" s="3"/>
+    </row>
+    <row r="482" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D482" s="3"/>
+    </row>
+    <row r="483" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D483" s="3"/>
+    </row>
+    <row r="484" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D484" s="3"/>
+    </row>
+    <row r="485" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D485" s="3"/>
+    </row>
+    <row r="486" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D486" s="3"/>
+    </row>
+    <row r="487" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D487" s="3"/>
+    </row>
+    <row r="488" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D488" s="3"/>
+    </row>
+    <row r="489" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D489" s="3"/>
+    </row>
+    <row r="490" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D490" s="3"/>
+    </row>
+    <row r="491" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D491" s="3"/>
+    </row>
+    <row r="492" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D492" s="3"/>
+    </row>
+    <row r="493" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D493" s="3"/>
+    </row>
+    <row r="494" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D494" s="3"/>
+    </row>
+    <row r="495" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D495" s="3"/>
+    </row>
+    <row r="496" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D496" s="3"/>
+    </row>
+    <row r="497" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D497" s="3"/>
+    </row>
+    <row r="498" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D498" s="3"/>
+    </row>
+    <row r="499" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D499" s="3"/>
+    </row>
+    <row r="500" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D500" s="3"/>
+    </row>
+    <row r="501" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D501" s="3"/>
+    </row>
+    <row r="502" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D502" s="3"/>
+    </row>
+    <row r="503" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D503" s="3"/>
+    </row>
+    <row r="504" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D504" s="3"/>
+    </row>
+    <row r="505" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D505" s="3"/>
+    </row>
+    <row r="506" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D506" s="3"/>
+    </row>
+    <row r="507" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D507" s="3"/>
+    </row>
+    <row r="508" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D508" s="3"/>
+    </row>
+    <row r="509" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D509" s="3"/>
+    </row>
+    <row r="510" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D510" s="3"/>
+    </row>
+    <row r="511" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D511" s="3"/>
+    </row>
+    <row r="512" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D512" s="3"/>
+    </row>
+    <row r="513" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D513" s="3"/>
+    </row>
+    <row r="514" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D514" s="3"/>
+    </row>
+    <row r="515" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D515" s="3"/>
+    </row>
+    <row r="516" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D516" s="3"/>
+    </row>
+    <row r="517" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D517" s="3"/>
+    </row>
+    <row r="518" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D518" s="3"/>
+    </row>
+    <row r="519" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D519" s="3"/>
+    </row>
+    <row r="520" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D520" s="3"/>
+    </row>
+    <row r="521" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D521" s="3"/>
+    </row>
+    <row r="522" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D522" s="3"/>
+    </row>
+    <row r="523" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D523" s="3"/>
+    </row>
+    <row r="524" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D524" s="3"/>
+    </row>
+    <row r="525" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D525" s="3"/>
+    </row>
+    <row r="526" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D526" s="3"/>
+    </row>
+    <row r="527" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D527" s="3"/>
+    </row>
+    <row r="528" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D528" s="3"/>
+    </row>
+    <row r="529" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D529" s="3"/>
+    </row>
+    <row r="530" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D530" s="3"/>
+    </row>
+    <row r="531" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D531" s="3"/>
+    </row>
+    <row r="532" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D532" s="3"/>
+    </row>
+    <row r="533" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D533" s="3"/>
+    </row>
+    <row r="534" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D534" s="3"/>
+    </row>
+    <row r="535" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D535" s="3"/>
+    </row>
+    <row r="536" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D536" s="3"/>
+    </row>
+    <row r="537" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D537" s="3"/>
+    </row>
+    <row r="538" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D538" s="3"/>
+    </row>
+    <row r="539" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D539" s="3"/>
+    </row>
+    <row r="540" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D540" s="3"/>
+    </row>
+    <row r="541" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D541" s="3"/>
+    </row>
+    <row r="542" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D542" s="3"/>
+    </row>
+    <row r="543" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D543" s="3"/>
+    </row>
+    <row r="544" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D544" s="3"/>
+    </row>
+    <row r="545" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D545" s="3"/>
+    </row>
+    <row r="546" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D546" s="3"/>
+    </row>
+    <row r="547" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D547" s="3"/>
+    </row>
+    <row r="548" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D548" s="3"/>
+    </row>
+    <row r="549" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D549" s="3"/>
+    </row>
+    <row r="550" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D550" s="3"/>
+    </row>
+    <row r="551" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D551" s="3"/>
+    </row>
+    <row r="552" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D552" s="3"/>
+    </row>
+    <row r="553" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D553" s="3"/>
+    </row>
+    <row r="554" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D554" s="3"/>
+    </row>
+    <row r="555" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D555" s="3"/>
+    </row>
+    <row r="556" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D556" s="3"/>
+    </row>
+    <row r="557" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D557" s="3"/>
+    </row>
+    <row r="558" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D558" s="3"/>
+    </row>
+    <row r="559" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D559" s="3"/>
+    </row>
+    <row r="560" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D560" s="3"/>
+    </row>
+    <row r="561" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D561" s="3"/>
+    </row>
+    <row r="562" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D562" s="3"/>
+    </row>
+    <row r="563" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D563" s="3"/>
+    </row>
+    <row r="564" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D564" s="3"/>
+    </row>
+    <row r="565" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D565" s="3"/>
+    </row>
+    <row r="566" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D566" s="3"/>
+    </row>
+    <row r="567" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D567" s="3"/>
+    </row>
+    <row r="568" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D568" s="3"/>
+    </row>
+    <row r="569" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D569" s="3"/>
+    </row>
+    <row r="570" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D570" s="3"/>
+    </row>
+    <row r="571" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D571" s="3"/>
+    </row>
+    <row r="572" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D572" s="3"/>
+    </row>
+    <row r="573" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D573" s="3"/>
+    </row>
+    <row r="574" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D574" s="3"/>
+    </row>
+    <row r="575" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D575" s="3"/>
+    </row>
+    <row r="576" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D576" s="3"/>
+    </row>
+    <row r="577" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D577" s="3"/>
+    </row>
+    <row r="578" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D578" s="3"/>
+    </row>
+    <row r="579" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D579" s="3"/>
+    </row>
+    <row r="580" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D580" s="3"/>
+    </row>
+    <row r="581" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D581" s="3"/>
+    </row>
+    <row r="582" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D582" s="3"/>
+    </row>
+    <row r="583" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D583" s="3"/>
+    </row>
+    <row r="584" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D584" s="3"/>
+    </row>
+    <row r="585" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D585" s="3"/>
+    </row>
+    <row r="586" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D586" s="3"/>
+    </row>
+    <row r="587" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D587" s="3"/>
+    </row>
+    <row r="588" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D588" s="3"/>
+    </row>
+    <row r="589" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D589" s="3"/>
+    </row>
+    <row r="590" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D590" s="3"/>
+    </row>
+    <row r="591" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D591" s="3"/>
+    </row>
+    <row r="592" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D592" s="3"/>
+    </row>
+    <row r="593" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D593" s="3"/>
+    </row>
+    <row r="594" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D594" s="3"/>
+    </row>
+    <row r="595" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D595" s="3"/>
+    </row>
+    <row r="596" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D596" s="3"/>
+    </row>
+    <row r="597" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D597" s="3"/>
+    </row>
+    <row r="598" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D598" s="3"/>
+    </row>
+    <row r="599" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D599" s="3"/>
+    </row>
+    <row r="600" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D600" s="3"/>
+    </row>
+    <row r="601" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D601" s="3"/>
+    </row>
+    <row r="602" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D602" s="3"/>
+    </row>
+    <row r="603" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D603" s="3"/>
+    </row>
+    <row r="604" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D604" s="3"/>
+    </row>
+    <row r="605" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D605" s="3"/>
+    </row>
+    <row r="606" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D606" s="3"/>
+    </row>
+    <row r="607" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D607" s="3"/>
+    </row>
+    <row r="608" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D608" s="3"/>
+    </row>
+    <row r="609" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D609" s="3"/>
+    </row>
+    <row r="610" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D610" s="3"/>
+    </row>
+    <row r="611" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D611" s="3"/>
+    </row>
+    <row r="612" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D612" s="3"/>
+    </row>
+    <row r="613" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D613" s="3"/>
+    </row>
+    <row r="614" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D614" s="3"/>
+    </row>
+    <row r="615" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D615" s="3"/>
+    </row>
+    <row r="616" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D616" s="3"/>
+    </row>
+    <row r="617" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D617" s="3"/>
+    </row>
+    <row r="618" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D618" s="3"/>
+    </row>
+    <row r="619" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D619" s="3"/>
+    </row>
+    <row r="620" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D620" s="3"/>
+    </row>
+    <row r="621" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D621" s="3"/>
+    </row>
+    <row r="622" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D622" s="3"/>
+    </row>
+    <row r="623" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D623" s="3"/>
+    </row>
+    <row r="624" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D624" s="3"/>
+    </row>
+    <row r="625" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D625" s="3"/>
+    </row>
+    <row r="626" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D626" s="3"/>
+    </row>
+    <row r="627" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D627" s="3"/>
+    </row>
+    <row r="628" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D628" s="3"/>
+    </row>
+    <row r="629" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D629" s="3"/>
+    </row>
+    <row r="630" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D630" s="3"/>
+    </row>
+    <row r="631" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D631" s="3"/>
+    </row>
+    <row r="632" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D632" s="3"/>
+    </row>
+    <row r="633" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D633" s="3"/>
+    </row>
+    <row r="634" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D634" s="3"/>
+    </row>
+    <row r="635" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D635" s="3"/>
+    </row>
+    <row r="636" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D636" s="3"/>
+    </row>
+    <row r="637" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D637" s="3"/>
+    </row>
+    <row r="638" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D638" s="3"/>
+    </row>
+    <row r="639" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D639" s="3"/>
+    </row>
+    <row r="640" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D640" s="3"/>
+    </row>
+    <row r="641" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D641" s="3"/>
+    </row>
+    <row r="642" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D642" s="3"/>
+    </row>
+    <row r="643" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D643" s="3"/>
+    </row>
+    <row r="644" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D644" s="3"/>
+    </row>
+    <row r="645" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D645" s="3"/>
+    </row>
+    <row r="646" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D646" s="3"/>
+    </row>
+    <row r="647" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D647" s="3"/>
+    </row>
+    <row r="648" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D648" s="3"/>
+    </row>
+    <row r="649" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D649" s="3"/>
+    </row>
+    <row r="650" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D650" s="3"/>
+    </row>
+    <row r="651" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D651" s="3"/>
+    </row>
+    <row r="652" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D652" s="3"/>
+    </row>
+    <row r="653" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D653" s="3"/>
+    </row>
+    <row r="654" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D654" s="3"/>
+    </row>
+    <row r="655" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D655" s="3"/>
+    </row>
+    <row r="656" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D656" s="3"/>
+    </row>
+    <row r="657" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D657" s="3"/>
+    </row>
+    <row r="658" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D658" s="3"/>
+    </row>
+    <row r="659" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D659" s="3"/>
+    </row>
+    <row r="660" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D660" s="3"/>
+    </row>
+    <row r="661" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D661" s="3"/>
+    </row>
+    <row r="662" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D662" s="3"/>
+    </row>
+    <row r="663" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D663" s="3"/>
+    </row>
+    <row r="664" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D664" s="3"/>
+    </row>
+    <row r="665" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D665" s="3"/>
+    </row>
+    <row r="666" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D666" s="3"/>
+    </row>
+    <row r="667" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D667" s="3"/>
+    </row>
+    <row r="668" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D668" s="3"/>
+    </row>
+    <row r="669" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D669" s="3"/>
+    </row>
+    <row r="670" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D670" s="3"/>
+    </row>
+    <row r="671" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D671" s="3"/>
+    </row>
+    <row r="672" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D672" s="3"/>
+    </row>
+    <row r="673" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D673" s="3"/>
+    </row>
+    <row r="674" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D674" s="3"/>
+    </row>
+    <row r="675" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D675" s="3"/>
+    </row>
+    <row r="676" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D676" s="3"/>
+    </row>
+    <row r="677" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D677" s="3"/>
+    </row>
+    <row r="678" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D678" s="3"/>
+    </row>
+    <row r="679" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D679" s="3"/>
+    </row>
+    <row r="680" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D680" s="3"/>
+    </row>
+    <row r="681" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D681" s="3"/>
+    </row>
+    <row r="682" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D682" s="3"/>
+    </row>
+    <row r="683" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D683" s="3"/>
+    </row>
+    <row r="684" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D684" s="3"/>
+    </row>
+    <row r="685" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D685" s="3"/>
+    </row>
+    <row r="686" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D686" s="3"/>
+    </row>
+    <row r="687" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D687" s="3"/>
+    </row>
+    <row r="688" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D688" s="3"/>
+    </row>
+    <row r="689" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D689" s="3"/>
+    </row>
+    <row r="690" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D690" s="3"/>
+    </row>
+    <row r="691" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D691" s="3"/>
+    </row>
+    <row r="692" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D692" s="3"/>
+    </row>
+    <row r="693" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D693" s="3"/>
+    </row>
+    <row r="694" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D694" s="3"/>
+    </row>
+    <row r="695" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D695" s="3"/>
+    </row>
+    <row r="696" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D696" s="3"/>
+    </row>
+    <row r="697" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D697" s="3"/>
+    </row>
+    <row r="698" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D698" s="3"/>
+    </row>
+    <row r="699" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D699" s="3"/>
+    </row>
+    <row r="700" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D700" s="3"/>
+    </row>
+    <row r="701" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D701" s="3"/>
+    </row>
+    <row r="702" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D702" s="3"/>
+    </row>
+    <row r="703" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D703" s="3"/>
+    </row>
+    <row r="704" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D704" s="3"/>
+    </row>
+    <row r="705" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D705" s="3"/>
+    </row>
+    <row r="706" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D706" s="3"/>
+    </row>
+    <row r="707" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D707" s="3"/>
+    </row>
+    <row r="708" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D708" s="3"/>
+    </row>
+    <row r="709" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D709" s="3"/>
+    </row>
+    <row r="710" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D710" s="3"/>
+    </row>
+    <row r="711" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D711" s="3"/>
+    </row>
+    <row r="712" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D712" s="3"/>
+    </row>
+    <row r="713" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D713" s="3"/>
+    </row>
+    <row r="714" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D714" s="3"/>
+    </row>
+    <row r="715" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D715" s="3"/>
+    </row>
+    <row r="716" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D716" s="3"/>
+    </row>
+    <row r="717" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D717" s="3"/>
+    </row>
+    <row r="718" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D718" s="3"/>
+    </row>
+    <row r="719" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D719" s="3"/>
+    </row>
+    <row r="720" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D720" s="3"/>
+    </row>
+    <row r="721" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D721" s="3"/>
+    </row>
+    <row r="722" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D722" s="3"/>
+    </row>
+    <row r="723" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D723" s="3"/>
+    </row>
+    <row r="724" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D724" s="3"/>
+    </row>
+    <row r="725" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D725" s="3"/>
+    </row>
+    <row r="726" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D726" s="3"/>
+    </row>
+    <row r="727" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D727" s="3"/>
+    </row>
+    <row r="728" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D728" s="3"/>
+    </row>
+    <row r="729" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D729" s="3"/>
+    </row>
+    <row r="730" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D730" s="3"/>
+    </row>
+    <row r="731" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D731" s="3"/>
+    </row>
+    <row r="732" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D732" s="3"/>
+    </row>
+    <row r="733" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D733" s="3"/>
+    </row>
+    <row r="734" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D734" s="3"/>
+    </row>
+    <row r="735" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D735" s="3"/>
+    </row>
+    <row r="736" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D736" s="3"/>
+    </row>
+    <row r="737" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D737" s="3"/>
+    </row>
+    <row r="738" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D738" s="3"/>
+    </row>
+    <row r="739" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D739" s="3"/>
+    </row>
+    <row r="740" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D740" s="3"/>
+    </row>
+    <row r="741" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D741" s="3"/>
+    </row>
+    <row r="742" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D742" s="3"/>
+    </row>
+    <row r="743" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D743" s="3"/>
+    </row>
+    <row r="744" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D744" s="3"/>
+    </row>
+    <row r="745" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D745" s="3"/>
+    </row>
+    <row r="746" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D746" s="3"/>
+    </row>
+    <row r="747" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D747" s="3"/>
+    </row>
+    <row r="748" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D748" s="3"/>
+    </row>
+    <row r="749" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D749" s="3"/>
+    </row>
+    <row r="750" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D750" s="3"/>
+    </row>
+    <row r="751" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D751" s="3"/>
+    </row>
+    <row r="752" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D752" s="3"/>
+    </row>
+    <row r="753" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D753" s="3"/>
+    </row>
+    <row r="754" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D754" s="3"/>
+    </row>
+    <row r="755" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D755" s="3"/>
+    </row>
+    <row r="756" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D756" s="3"/>
+    </row>
+    <row r="757" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D757" s="3"/>
+    </row>
+    <row r="758" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D758" s="3"/>
+    </row>
+    <row r="759" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D759" s="3"/>
+    </row>
+    <row r="760" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D760" s="3"/>
+    </row>
+    <row r="761" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D761" s="3"/>
+    </row>
+    <row r="762" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D762" s="3"/>
+    </row>
+    <row r="763" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D763" s="3"/>
+    </row>
+    <row r="764" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D764" s="3"/>
+    </row>
+    <row r="765" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D765" s="3"/>
+    </row>
+    <row r="766" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D766" s="3"/>
+    </row>
+    <row r="767" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D767" s="3"/>
+    </row>
+    <row r="768" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D768" s="3"/>
+    </row>
+    <row r="769" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D769" s="3"/>
+    </row>
+    <row r="770" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D770" s="3"/>
+    </row>
+    <row r="771" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D771" s="3"/>
+    </row>
+    <row r="772" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D772" s="3"/>
+    </row>
+    <row r="773" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D773" s="3"/>
+    </row>
+    <row r="774" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D774" s="3"/>
+    </row>
+    <row r="775" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D775" s="3"/>
+    </row>
+    <row r="776" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D776" s="3"/>
+    </row>
+    <row r="777" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D777" s="3"/>
+    </row>
+    <row r="778" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D778" s="3"/>
+    </row>
+    <row r="779" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D779" s="3"/>
+    </row>
+    <row r="780" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D780" s="3"/>
+    </row>
+    <row r="781" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D781" s="3"/>
+    </row>
+    <row r="782" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D782" s="3"/>
+    </row>
+    <row r="783" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D783" s="3"/>
+    </row>
+    <row r="784" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D784" s="3"/>
+    </row>
+    <row r="785" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D785" s="3"/>
+    </row>
+    <row r="786" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D786" s="3"/>
+    </row>
+    <row r="787" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D787" s="3"/>
+    </row>
+    <row r="788" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D788" s="3"/>
+    </row>
+    <row r="789" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D789" s="3"/>
+    </row>
+    <row r="790" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D790" s="3"/>
+    </row>
+    <row r="791" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D791" s="3"/>
+    </row>
+    <row r="792" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D792" s="3"/>
+    </row>
+    <row r="793" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D793" s="3"/>
+    </row>
+    <row r="794" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D794" s="3"/>
+    </row>
+    <row r="795" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D795" s="3"/>
+    </row>
+    <row r="796" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D796" s="3"/>
+    </row>
+    <row r="797" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D797" s="3"/>
+    </row>
+    <row r="798" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D798" s="3"/>
+    </row>
+    <row r="799" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D799" s="3"/>
+    </row>
+    <row r="800" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D800" s="3"/>
+    </row>
+    <row r="801" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D801" s="3"/>
+    </row>
+    <row r="802" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D802" s="3"/>
+    </row>
+    <row r="803" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D803" s="3"/>
+    </row>
+    <row r="804" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D804" s="3"/>
+    </row>
+    <row r="805" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D805" s="3"/>
+    </row>
+    <row r="806" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D806" s="3"/>
+    </row>
+    <row r="807" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D807" s="3"/>
+    </row>
+    <row r="808" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D808" s="3"/>
+    </row>
+    <row r="809" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D809" s="3"/>
+    </row>
+    <row r="810" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D810" s="3"/>
+    </row>
+    <row r="811" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D811" s="3"/>
+    </row>
+    <row r="812" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D812" s="3"/>
+    </row>
+    <row r="813" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D813" s="3"/>
+    </row>
+    <row r="814" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D814" s="3"/>
+    </row>
+    <row r="815" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D815" s="3"/>
+    </row>
+    <row r="816" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D816" s="3"/>
+    </row>
+    <row r="817" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D817" s="3"/>
+    </row>
+    <row r="818" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D818" s="3"/>
+    </row>
+    <row r="819" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D819" s="3"/>
+    </row>
+    <row r="820" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D820" s="3"/>
+    </row>
+    <row r="821" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D821" s="3"/>
+    </row>
+    <row r="822" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D822" s="3"/>
+    </row>
+    <row r="823" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D823" s="3"/>
+    </row>
+    <row r="824" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D824" s="3"/>
+    </row>
+    <row r="825" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D825" s="3"/>
+    </row>
+    <row r="826" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D826" s="3"/>
+    </row>
+    <row r="827" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D827" s="3"/>
+    </row>
+    <row r="828" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D828" s="3"/>
+    </row>
+    <row r="829" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D829" s="3"/>
+    </row>
+    <row r="830" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D830" s="3"/>
+    </row>
+    <row r="831" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D831" s="3"/>
+    </row>
+    <row r="832" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D832" s="3"/>
+    </row>
+    <row r="833" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D833" s="3"/>
+    </row>
+    <row r="834" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D834" s="3"/>
+    </row>
+    <row r="835" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D835" s="3"/>
+    </row>
+    <row r="836" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D836" s="3"/>
+    </row>
+    <row r="837" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D837" s="3"/>
+    </row>
+    <row r="838" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D838" s="3"/>
+    </row>
+    <row r="839" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D839" s="3"/>
+    </row>
+    <row r="840" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D840" s="3"/>
+    </row>
+    <row r="841" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D841" s="3"/>
+    </row>
+    <row r="842" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D842" s="3"/>
+    </row>
+    <row r="843" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D843" s="3"/>
+    </row>
+    <row r="844" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D844" s="3"/>
+    </row>
+    <row r="845" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D845" s="3"/>
+    </row>
+    <row r="846" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D846" s="3"/>
+    </row>
+    <row r="847" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D847" s="3"/>
+    </row>
+    <row r="848" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D848" s="3"/>
+    </row>
+    <row r="849" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D849" s="3"/>
+    </row>
+    <row r="850" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D850" s="3"/>
+    </row>
+    <row r="851" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D851" s="3"/>
+    </row>
+    <row r="852" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D852" s="3"/>
+    </row>
+    <row r="853" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D853" s="3"/>
+    </row>
+    <row r="854" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D854" s="3"/>
+    </row>
+    <row r="855" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D855" s="3"/>
+    </row>
+    <row r="856" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D856" s="3"/>
+    </row>
+    <row r="857" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D857" s="3"/>
+    </row>
+    <row r="858" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D858" s="3"/>
+    </row>
+    <row r="859" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D859" s="3"/>
+    </row>
+    <row r="860" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D860" s="3"/>
+    </row>
+    <row r="861" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D861" s="3"/>
+    </row>
+    <row r="862" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D862" s="3"/>
+    </row>
+    <row r="863" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D863" s="3"/>
+    </row>
+    <row r="864" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D864" s="3"/>
+    </row>
+    <row r="865" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D865" s="3"/>
+    </row>
+    <row r="866" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D866" s="3"/>
+    </row>
+    <row r="867" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D867" s="3"/>
+    </row>
+    <row r="868" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D868" s="3"/>
+    </row>
+    <row r="869" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D869" s="3"/>
+    </row>
+    <row r="870" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D870" s="3"/>
+    </row>
+    <row r="871" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D871" s="3"/>
+    </row>
+    <row r="872" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D872" s="3"/>
+    </row>
+    <row r="873" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D873" s="3"/>
+    </row>
+    <row r="874" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D874" s="3"/>
+    </row>
+    <row r="875" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D875" s="3"/>
+    </row>
+    <row r="876" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D876" s="3"/>
+    </row>
+    <row r="877" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D877" s="3"/>
+    </row>
+    <row r="878" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D878" s="3"/>
+    </row>
+    <row r="879" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D879" s="3"/>
+    </row>
+    <row r="880" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D880" s="3"/>
+    </row>
+    <row r="881" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D881" s="3"/>
+    </row>
+    <row r="882" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D882" s="3"/>
+    </row>
+    <row r="883" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D883" s="3"/>
+    </row>
+    <row r="884" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D884" s="3"/>
+    </row>
+    <row r="885" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D885" s="3"/>
+    </row>
+    <row r="886" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D886" s="3"/>
+    </row>
+    <row r="887" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D887" s="3"/>
+    </row>
+    <row r="888" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D888" s="3"/>
+    </row>
+    <row r="889" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D889" s="3"/>
+    </row>
+    <row r="890" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D890" s="3"/>
+    </row>
+    <row r="891" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D891" s="3"/>
+    </row>
+    <row r="892" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D892" s="3"/>
+    </row>
+    <row r="893" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D893" s="3"/>
+    </row>
+    <row r="894" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D894" s="3"/>
+    </row>
+    <row r="895" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D895" s="3"/>
+    </row>
+    <row r="896" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D896" s="3"/>
+    </row>
+    <row r="897" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D897" s="3"/>
+    </row>
+    <row r="898" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D898" s="3"/>
+    </row>
+    <row r="899" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D899" s="3"/>
+    </row>
+    <row r="900" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D900" s="3"/>
+    </row>
+    <row r="901" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D901" s="3"/>
+    </row>
+    <row r="902" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D902" s="3"/>
+    </row>
+    <row r="903" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D903" s="3"/>
+    </row>
+    <row r="904" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D904" s="3"/>
+    </row>
+    <row r="905" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D905" s="3"/>
+    </row>
+    <row r="906" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D906" s="3"/>
+    </row>
+    <row r="907" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D907" s="3"/>
+    </row>
+    <row r="908" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D908" s="3"/>
+    </row>
+    <row r="909" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D909" s="3"/>
+    </row>
+    <row r="910" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D910" s="3"/>
+    </row>
+    <row r="911" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D911" s="3"/>
+    </row>
+    <row r="912" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D912" s="3"/>
+    </row>
+    <row r="913" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D913" s="3"/>
+    </row>
+    <row r="914" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D914" s="3"/>
+    </row>
+    <row r="915" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D915" s="3"/>
+    </row>
+    <row r="916" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D916" s="3"/>
+    </row>
+    <row r="917" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D917" s="3"/>
+    </row>
+    <row r="918" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D918" s="3"/>
+    </row>
+    <row r="919" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D919" s="3"/>
+    </row>
+    <row r="920" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D920" s="3"/>
+    </row>
+    <row r="921" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D921" s="3"/>
+    </row>
+    <row r="922" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D922" s="3"/>
+    </row>
+    <row r="923" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D923" s="3"/>
+    </row>
+    <row r="924" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D924" s="3"/>
+    </row>
+    <row r="925" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D925" s="3"/>
+    </row>
+    <row r="926" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D926" s="3"/>
+    </row>
+    <row r="927" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D927" s="3"/>
+    </row>
+    <row r="928" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D928" s="3"/>
+    </row>
+    <row r="929" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D929" s="3"/>
+    </row>
+    <row r="930" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D930" s="3"/>
+    </row>
+    <row r="931" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D931" s="3"/>
+    </row>
+    <row r="932" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D932" s="3"/>
+    </row>
+    <row r="933" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D933" s="3"/>
+    </row>
+    <row r="934" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D934" s="3"/>
+    </row>
+    <row r="935" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D935" s="3"/>
+    </row>
+    <row r="936" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D936" s="3"/>
+    </row>
+    <row r="937" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D937" s="3"/>
+    </row>
+    <row r="938" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D938" s="3"/>
+    </row>
+    <row r="939" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D939" s="3"/>
+    </row>
+    <row r="940" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D940" s="3"/>
+    </row>
+    <row r="941" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D941" s="3"/>
+    </row>
+    <row r="942" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D942" s="3"/>
+    </row>
+    <row r="943" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D943" s="3"/>
+    </row>
+    <row r="944" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D944" s="3"/>
+    </row>
+    <row r="945" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D945" s="3"/>
+    </row>
+    <row r="946" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D946" s="3"/>
+    </row>
+    <row r="947" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D947" s="3"/>
+    </row>
+    <row r="948" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D948" s="3"/>
+    </row>
+    <row r="949" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D949" s="3"/>
+    </row>
+    <row r="950" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D950" s="3"/>
+    </row>
+    <row r="951" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D951" s="3"/>
+    </row>
+    <row r="952" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D952" s="3"/>
+    </row>
+    <row r="953" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D953" s="3"/>
+    </row>
+    <row r="954" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D954" s="3"/>
+    </row>
+    <row r="955" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D955" s="3"/>
+    </row>
+    <row r="956" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D956" s="3"/>
+    </row>
+    <row r="957" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D957" s="3"/>
+    </row>
+    <row r="958" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D958" s="3"/>
+    </row>
+    <row r="959" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D959" s="3"/>
+    </row>
+    <row r="960" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D960" s="3"/>
+    </row>
+    <row r="961" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D961" s="3"/>
+    </row>
+    <row r="962" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D962" s="3"/>
+    </row>
+    <row r="963" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D963" s="3"/>
+    </row>
+    <row r="964" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D964" s="3"/>
+    </row>
+    <row r="965" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D965" s="3"/>
+    </row>
+    <row r="966" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D966" s="3"/>
+    </row>
+    <row r="967" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D967" s="3"/>
+    </row>
+    <row r="968" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D968" s="3"/>
+    </row>
+    <row r="969" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D969" s="3"/>
+    </row>
+    <row r="970" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D970" s="3"/>
+    </row>
+    <row r="971" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D971" s="3"/>
+    </row>
+    <row r="972" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D972" s="3"/>
+    </row>
+    <row r="973" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D973" s="3"/>
+    </row>
+    <row r="974" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D974" s="3"/>
+    </row>
+    <row r="975" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D975" s="3"/>
+    </row>
+    <row r="976" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D976" s="3"/>
+    </row>
+    <row r="977" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D977" s="3"/>
+    </row>
+    <row r="978" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D978" s="3"/>
+    </row>
+    <row r="979" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D979" s="3"/>
+    </row>
+    <row r="980" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D980" s="3"/>
+    </row>
+    <row r="981" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D981" s="3"/>
+    </row>
+    <row r="982" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D982" s="3"/>
+    </row>
+    <row r="983" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D983" s="3"/>
+    </row>
+    <row r="984" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D984" s="3"/>
+    </row>
+    <row r="985" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D985" s="3"/>
+    </row>
+    <row r="986" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D986" s="3"/>
+    </row>
+    <row r="987" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D987" s="3"/>
+    </row>
+    <row r="988" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D988" s="3"/>
+    </row>
+    <row r="989" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D989" s="3"/>
+    </row>
+    <row r="990" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D990" s="3"/>
+    </row>
+    <row r="991" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D991" s="3"/>
+    </row>
+    <row r="992" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D992" s="3"/>
+    </row>
+    <row r="993" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D993" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L985"/>
   <sheetViews>
@@ -20083,7 +23320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK64"/>
   <sheetViews>
@@ -22600,7 +25837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K1005"/>
   <sheetViews>

</xml_diff>

<commit_message>
VIP and Cryosleep Imputation Completed
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10BAA5F-F150-4F0F-BED7-59A9DD2AD79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C78480-C58C-464E-9E75-340E01E93D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="127">
   <si>
     <t>Version</t>
   </si>
@@ -413,10 +413,19 @@
     <t>Start Titanic 3.0.4 Cabin Deck</t>
   </si>
   <si>
-    <t>Cabin Side</t>
+    <t>Titanic 6.0.0</t>
   </si>
   <si>
-    <t>Titanic 6.0.0</t>
+    <t>Titanic 6.0.1</t>
+  </si>
+  <si>
+    <t>2024 08 18</t>
+  </si>
+  <si>
+    <t>Start Titanic 3.0.7 Cabin Side</t>
+  </si>
+  <si>
+    <t>Start Titanic 3.0.8 Cabin Number</t>
   </si>
 </sst>
 </file>
@@ -7321,8 +7330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
   <dimension ref="A1:L993"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17011,10 +17020,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6254EBB-BCB6-46DB-AD5A-C24358141626}">
-  <dimension ref="A1:L993"/>
+  <dimension ref="A1:L994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A12" sqref="A12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17044,7 +17053,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>115</v>
@@ -17108,37 +17117,49 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>122</v>
+      <c r="D8" s="3"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>123</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -17277,43 +17298,45 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="3"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="B34" s="5"/>
       <c r="D34" s="3"/>
-      <c r="G34" s="8"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="B37" s="5"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
@@ -17333,28 +17356,29 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
-      <c r="B42" s="6"/>
+      <c r="B42" s="5"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="6"/>
       <c r="D43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="3"/>
+      <c r="B44" s="5"/>
       <c r="D44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="3"/>
-      <c r="B46" s="5"/>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
       <c r="B47" s="5"/>
       <c r="D47" s="3"/>
     </row>
@@ -17383,6 +17407,7 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B54" s="5"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.35">
@@ -20201,6 +20226,9 @@
     </row>
     <row r="993" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D993" s="3"/>
+    </row>
+    <row r="994" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D994" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Titanic 7.0.0 Encoding and Scaling
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5129FBF2-08D1-4FE0-A909-2387015B84D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A61264-CF85-4915-943C-8D817396DF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
   <si>
     <t>Version</t>
   </si>
@@ -446,6 +446,18 @@
   </si>
   <si>
     <t>Start Titanic 6.0.2</t>
+  </si>
+  <si>
+    <t>Titanic 5.0.1</t>
+  </si>
+  <si>
+    <t>Titaninc 5.0.2</t>
+  </si>
+  <si>
+    <t>Concatenated Train and Test Data in a different way.</t>
+  </si>
+  <si>
+    <t>2024 08 19</t>
   </si>
 </sst>
 </file>
@@ -10663,7 +10675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
   <dimension ref="A1:L993"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -17155,10 +17167,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBBBD00-887E-4CE6-9C0B-B6A8EADE2E47}">
-  <dimension ref="A1:L994"/>
+  <dimension ref="A1:L995"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17220,35 +17232,35 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>114</v>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>133</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
@@ -17256,19 +17268,31 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="5"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -17428,43 +17452,45 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="6"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="3"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="5"/>
       <c r="D35" s="3"/>
-      <c r="G35" s="8"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="3"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="B38" s="5"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -17484,28 +17510,29 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
-      <c r="B43" s="6"/>
+      <c r="B43" s="5"/>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
-      <c r="B44" s="5"/>
+      <c r="B44" s="6"/>
       <c r="D44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="5"/>
       <c r="D45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="5"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="3"/>
       <c r="B48" s="5"/>
       <c r="D48" s="3"/>
     </row>
@@ -17534,6 +17561,7 @@
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B55" s="5"/>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.35">
@@ -20352,6 +20380,9 @@
     </row>
     <row r="994" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D994" s="3"/>
+    </row>
+    <row r="995" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D995" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -20363,7 +20394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6254EBB-BCB6-46DB-AD5A-C24358141626}">
   <dimension ref="A1:L994"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -23596,7 +23627,7 @@
   <dimension ref="A1:L994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23631,9 +23662,7 @@
       <c r="B2" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>124</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
Completed Model Selection (Titanic 7.0.2)
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C0D156-DE30-4286-90EB-FCBBD7D922FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB32DE8E-3A39-4378-AB2D-845169CC850C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extraction 1.0" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="148">
   <si>
     <t>Version</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>Wine Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.describe </t>
   </si>
   <si>
     <t>AUC is more robust than precision and recall</t>
@@ -459,6 +456,42 @@
   <si>
     <t>2024 08 19</t>
   </si>
+  <si>
+    <t>Titanic 7.0.1</t>
+  </si>
+  <si>
+    <t>2024 08 21</t>
+  </si>
+  <si>
+    <t>2024 08 20</t>
+  </si>
+  <si>
+    <t>Start ML: Logistic Regression and others</t>
+  </si>
+  <si>
+    <t>CAT BOOST doesn't work.</t>
+  </si>
+  <si>
+    <t>Titanic 7.0.2</t>
+  </si>
+  <si>
+    <t>2024 08 22</t>
+  </si>
+  <si>
+    <t>Started newevn virtual environment.</t>
+  </si>
+  <si>
+    <t>Started FRESH spaceenv to test issue with CAT Boost</t>
+  </si>
+  <si>
+    <t>Use Windows Command in Administrative Mode.</t>
+  </si>
+  <si>
+    <t>Windows Prompt</t>
+  </si>
+  <si>
+    <t>Use it in administrative mode to add librarires.</t>
+  </si>
 </sst>
 </file>
 
@@ -468,7 +501,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]#,##0.00_);\(#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;\-#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -512,13 +545,26 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF323232"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="186"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -544,7 +590,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -591,6 +637,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,46 +1114,46 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
@@ -1103,16 +1161,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -1121,7 +1179,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1130,7 +1188,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -4185,10 +4243,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K1002"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4215,7 +4273,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="17"/>
     </row>
@@ -4227,7 +4285,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -4250,7 +4308,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3"/>
       <c r="F6" s="5"/>
@@ -4263,7 +4321,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="3"/>
@@ -4280,7 +4338,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3"/>
       <c r="F9" s="5"/>
@@ -4308,7 +4366,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3"/>
       <c r="F12" s="5"/>
@@ -4357,7 +4415,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -4370,7 +4428,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3"/>
       <c r="F19" s="5"/>
@@ -4394,7 +4452,7 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3"/>
       <c r="F22" s="5"/>
@@ -4435,7 +4493,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -4455,11 +4513,11 @@
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="3"/>
-      <c r="F30" s="5"/>
+    <row r="30" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
@@ -4471,10 +4529,10 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
-      <c r="B32" s="15"/>
-      <c r="F32" s="5"/>
+    <row r="32" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="F32" s="24"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
@@ -4494,77 +4552,77 @@
       </c>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="13">
-        <v>6</v>
-      </c>
-      <c r="F35" s="5"/>
+    <row r="35" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="15" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
-      <c r="C36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
-      <c r="B37" s="15"/>
+      <c r="B37" s="25" t="s">
+        <v>28</v>
+      </c>
       <c r="C37" s="3"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
-      <c r="B38" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38" s="5"/>
+    <row r="38" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="20"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
+      <c r="F38" s="24"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="15" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C39" s="3"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
-      <c r="B41" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B41" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="5"/>
+      <c r="C41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="20"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
-      <c r="B43" s="16" t="s">
-        <v>60</v>
+      <c r="B43" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>61</v>
+        <v>147</v>
       </c>
-      <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="13"/>
@@ -4600,28 +4658,26 @@
       <c r="A50" s="13"/>
       <c r="B50" s="15"/>
       <c r="C50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="5"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" s="13"/>
       <c r="B51" s="15"/>
       <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="13"/>
-      <c r="B52" s="15"/>
       <c r="C52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="5"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B53" s="15"/>
+      <c r="A53" s="13"/>
       <c r="C53" s="3"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B54" s="15"/>
       <c r="C54" s="3"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A55" s="13"/>
+      <c r="B55" s="15"/>
       <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
@@ -4649,11 +4705,9 @@
       <c r="C61" s="3"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B62" s="15"/>
       <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B63" s="15"/>
       <c r="C63" s="3"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
@@ -7466,12 +7520,6 @@
     </row>
     <row r="1000" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C1000" s="3"/>
-    </row>
-    <row r="1001" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C1001" s="3"/>
-    </row>
-    <row r="1002" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C1002" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7514,46 +7562,46 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>65</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>66</v>
+      <c r="C3" s="3" t="s">
+        <v>54</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
@@ -7561,46 +7609,46 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>67</v>
+      <c r="C6" s="3" t="s">
+        <v>68</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -10689,16 +10737,16 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -10707,7 +10755,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -10716,7 +10764,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G4" s="5"/>
     </row>
@@ -10729,16 +10777,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="3"/>
@@ -10749,7 +10797,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -10758,7 +10806,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -10771,16 +10819,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -10789,7 +10837,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -10798,7 +10846,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -10811,16 +10859,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -10829,7 +10877,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -10842,16 +10890,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" s="5"/>
     </row>
@@ -10860,7 +10908,7 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" s="5"/>
     </row>
@@ -10869,7 +10917,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" s="5"/>
     </row>
@@ -10882,16 +10930,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G21" s="5"/>
     </row>
@@ -10900,7 +10948,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G22" s="5"/>
     </row>
@@ -10913,16 +10961,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G24" s="5"/>
     </row>
@@ -10931,7 +10979,7 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" s="5"/>
     </row>
@@ -10944,16 +10992,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G27" s="5"/>
     </row>
@@ -10962,7 +11010,7 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G28" s="5"/>
     </row>
@@ -10975,31 +11023,31 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G31" s="5"/>
     </row>
@@ -11008,7 +11056,7 @@
       <c r="B32" s="3"/>
       <c r="C32" s="6"/>
       <c r="D32" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G32" s="5"/>
     </row>
@@ -11020,16 +11068,16 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G34" s="8"/>
     </row>
@@ -11038,7 +11086,7 @@
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
@@ -11048,23 +11096,23 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="5"/>
       <c r="D38" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
@@ -13989,21 +14037,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="B2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -14012,7 +14060,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -17178,21 +17226,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -17201,7 +17249,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -17210,7 +17258,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="5"/>
     </row>
@@ -17223,16 +17271,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -17241,7 +17289,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -17256,16 +17304,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -17274,7 +17322,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -20403,21 +20451,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -20426,7 +20474,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -20435,7 +20483,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="5"/>
     </row>
@@ -20444,7 +20492,7 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -20453,7 +20501,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="3"/>
@@ -20464,7 +20512,7 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -20477,16 +20525,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -20495,7 +20543,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -20504,7 +20552,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -20513,7 +20561,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -20526,16 +20574,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -20544,7 +20592,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -20553,7 +20601,7 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G16" s="5"/>
     </row>
@@ -20562,7 +20610,7 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" s="5"/>
     </row>
@@ -23610,7 +23658,7 @@
   <dimension ref="A1:L994"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23635,19 +23683,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -23655,28 +23705,48 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="G6" s="5"/>
       <c r="H6" s="3"/>
       <c r="I6" s="5"/>
@@ -23685,7 +23755,9 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Titanic EDA 2.0.1 Modified
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BD9F2F-3111-43D9-B88E-01876EF8760C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AB51B3-DDE9-4D65-A23A-316CB3C9FD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extraction 1.0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Preprocess 5.0" sheetId="8" r:id="rId5"/>
     <sheet name="Missing 6.0" sheetId="9" r:id="rId6"/>
     <sheet name="ML 7.0" sheetId="10" r:id="rId7"/>
-    <sheet name="Final" sheetId="11" r:id="rId8"/>
+    <sheet name="Project" sheetId="11" r:id="rId8"/>
     <sheet name="Pipelines" sheetId="3" r:id="rId9"/>
     <sheet name="Alert" sheetId="4" state="hidden" r:id="rId10"/>
     <sheet name="Ideas" sheetId="5" r:id="rId11"/>
@@ -29,7 +29,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="9">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="7">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="10">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -37,6 +36,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="8">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="7">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="164">
   <si>
     <t>Version</t>
   </si>
@@ -507,9 +507,6 @@
     <t>Titanic 7.0.3</t>
   </si>
   <si>
-    <t>Add Correlation between features</t>
-  </si>
-  <si>
     <t>Consider other types of encoders: Target, WOEEncoder</t>
   </si>
   <si>
@@ -519,13 +516,31 @@
     <t>F1-score or PR AUC</t>
   </si>
   <si>
-    <t>Spearman correlation</t>
-  </si>
-  <si>
     <t>Repeated Code</t>
   </si>
   <si>
     <t>Other types of scaling</t>
+  </si>
+  <si>
+    <t>black formatter: Long lines</t>
+  </si>
+  <si>
+    <t>PEP 8</t>
+  </si>
+  <si>
+    <t>PyLint</t>
+  </si>
+  <si>
+    <t>Titanic 7.0.5</t>
+  </si>
+  <si>
+    <t>2024 08 26</t>
+  </si>
+  <si>
+    <t>Final checks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revising </t>
   </si>
 </sst>
 </file>
@@ -26254,7 +26269,7 @@
   <dimension ref="A1:L995"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -26397,10 +26412,18 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:9">
@@ -29486,10 +29509,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D055CC6A-9AD8-4AB0-8C32-BFB14E983AA1}">
-  <dimension ref="A1:L995"/>
+  <dimension ref="A1:L993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -29503,7 +29526,7 @@
     <col min="8" max="1025" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:7" ht="15" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -29517,7 +29540,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1">
+    <row r="2" spans="1:7" ht="15" thickTop="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -29526,7 +29549,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -29535,25 +29558,25 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="36" t="s">
         <v>154</v>
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="3" t="s">
         <v>155</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:7">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -29561,10 +29584,8 @@
         <v>156</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -29573,65 +29594,75 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:7">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="3" t="s">
         <v>158</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:7">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:7">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:7">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:7">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -29746,41 +29777,38 @@
     <row r="32" spans="1:7">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="3"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="B33" s="5"/>
       <c r="D33" s="3"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="6"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="G34" s="5"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="3"/>
-      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="B36" s="5"/>
       <c r="D36" s="3"/>
-      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="3"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:12">
@@ -29790,8 +29818,7 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="B39" s="5"/>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:12">
@@ -29806,34 +29833,32 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="6"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="3"/>
       <c r="B43" s="5"/>
       <c r="D43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="3"/>
-      <c r="B44" s="6"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="3"/>
-      <c r="B45" s="5"/>
       <c r="D45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12">
+      <c r="A46" s="3"/>
+      <c r="B46" s="5"/>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:12">
+      <c r="B47" s="5"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="3"/>
       <c r="B48" s="5"/>
       <c r="D48" s="3"/>
     </row>
@@ -29858,11 +29883,9 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" s="5"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="2:4">
-      <c r="B55" s="5"/>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="2:4">
@@ -32678,12 +32701,6 @@
     </row>
     <row r="993" spans="4:4">
       <c r="D993" s="3"/>
-    </row>
-    <row r="994" spans="4:4">
-      <c r="D994" s="3"/>
-    </row>
-    <row r="995" spans="4:4">
-      <c r="D995" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Insights Added: Overview Notebook.
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02279D89-FD4E-4108-9BB5-2F3A5A59D958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41EF5A3-04B4-4A91-89D2-8482EBAD292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="167">
   <si>
     <t>Version</t>
   </si>
@@ -29518,10 +29518,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D055CC6A-9AD8-4AB0-8C32-BFB14E983AA1}">
-  <dimension ref="A1:L993"/>
+  <dimension ref="A1:L994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -29622,54 +29622,56 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7">
@@ -29794,43 +29796,45 @@
     <row r="32" spans="1:7">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="3"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="B34" s="5"/>
       <c r="D34" s="3"/>
-      <c r="G34" s="8"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="B37" s="5"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="3"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12">
@@ -29850,28 +29854,29 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="3"/>
-      <c r="B42" s="6"/>
+      <c r="B42" s="5"/>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="3"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="6"/>
       <c r="D43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12">
+      <c r="A44" s="3"/>
+      <c r="B44" s="5"/>
       <c r="D44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12">
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="3"/>
-      <c r="B46" s="5"/>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:12">
+      <c r="A47" s="3"/>
       <c r="B47" s="5"/>
       <c r="D47" s="3"/>
     </row>
@@ -29900,6 +29905,7 @@
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="2:4">
+      <c r="B54" s="5"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="2:4">
@@ -32718,6 +32724,9 @@
     </row>
     <row r="993" spans="4:4">
       <c r="D993" s="3"/>
+    </row>
+    <row r="994" spans="4:4">
+      <c r="D994" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Completed Comments on Missing Values Notebook
</commit_message>
<xml_diff>
--- a/Documentation/Titanic.xlsx
+++ b/Documentation/Titanic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Titanic\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41EF5A3-04B4-4A91-89D2-8482EBAD292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECD894A-08A4-47EC-B820-3E1A44664F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Extraction 1.0" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="172">
   <si>
     <t>Version</t>
   </si>
@@ -550,6 +550,21 @@
   </si>
   <si>
     <t>2024 08 27</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Add heatmap</t>
+  </si>
+  <si>
+    <t>Titanic EDA 2.0.2</t>
+  </si>
+  <si>
+    <t>2024 08 28</t>
+  </si>
+  <si>
+    <t>Adding insights.</t>
   </si>
 </sst>
 </file>
@@ -10149,15 +10164,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L986"/>
+  <dimension ref="A1:L989"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.08984375" customWidth="1"/>
     <col min="3" max="3" width="8.453125" customWidth="1"/>
     <col min="4" max="4" width="141" customWidth="1"/>
@@ -10280,17 +10295,27 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:9">
@@ -10301,10 +10326,18 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>171</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:9">
@@ -10386,20 +10419,22 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3"/>
-      <c r="B24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="6"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="G26" s="5"/>
     </row>
@@ -10407,13 +10442,14 @@
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
       <c r="D27" s="3"/>
-      <c r="G27" s="8"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="3"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="6"/>
       <c r="D28" s="3"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3"/>
@@ -10427,7 +10463,8 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:7">
@@ -10447,20 +10484,24 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3"/>
-      <c r="B35" s="6"/>
+      <c r="B35" s="5"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3"/>
       <c r="B36" s="5"/>
       <c r="D36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12">
+      <c r="A37" s="3"/>
+      <c r="B37" s="5"/>
       <c r="D37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12">
+      <c r="A38" s="3"/>
+      <c r="B38" s="6"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:12">
@@ -10469,14 +10510,13 @@
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="B40" s="5"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="B41" s="5"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:12">
+      <c r="A42" s="3"/>
       <c r="B42" s="5"/>
       <c r="D42" s="3"/>
     </row>
@@ -10497,57 +10537,60 @@
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:12">
+      <c r="B47" s="5"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:12">
+      <c r="B48" s="5"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="2:4">
+      <c r="B49" s="5"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="2:4">
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="2:4">
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="2:4">
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="2:4">
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="2:4">
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="2:4">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="2:4">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="2:4">
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="2:4">
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="2:4">
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="2:4">
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="2:4">
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="2:4">
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="2:4">
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="2:4">
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="4:4">
@@ -13315,6 +13358,15 @@
     </row>
     <row r="986" spans="4:4">
       <c r="D986" s="3"/>
+    </row>
+    <row r="987" spans="4:4">
+      <c r="D987" s="3"/>
+    </row>
+    <row r="988" spans="4:4">
+      <c r="D988" s="3"/>
+    </row>
+    <row r="989" spans="4:4">
+      <c r="D989" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -13326,7 +13378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67423FF-E569-4F35-927A-1F27FDA5B988}">
   <dimension ref="A1:L993"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -19821,7 +19873,7 @@
   <dimension ref="A1:L995"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -19957,14 +20009,18 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:9">
@@ -29520,8 +29576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D055CC6A-9AD8-4AB0-8C32-BFB14E983AA1}">
   <dimension ref="A1:L994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -29651,27 +29707,9 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7">

</xml_diff>